<commit_message>
removed references to missing images. Modified makefile to clean docs/ folder
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -581,6 +581,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -877,7 +878,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,7 +917,7 @@
         <v>Cerebro PCB</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(cerebro_data!C2),"",CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`Cerebro 5.4&lt;Datasheets/cerebro5.4.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
@@ -934,7 +935,7 @@
         <v>400 mAh Battery</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(cerebro_data!C3),"",CONCATENATE(" :download:`",cerebro_data!C3,"&lt;Datasheets/",cerebro_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D3),cerebro_data!C3,CONCATENATE(" :download:`",cerebro_data!C3,"&lt;Datasheets/",cerebro_data!D3,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`1570&lt;Datasheets/battery_400mah.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
@@ -952,7 +953,7 @@
         <v>915 MHz Radio</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(cerebro_data!C4),"",CONCATENATE(" :download:`",cerebro_data!C4,"&lt;Datasheets/",cerebro_data!D4,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D4),cerebro_data!C4,CONCATENATE(" :download:`",cerebro_data!C4,"&lt;Datasheets/",cerebro_data!D4,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`RFM69HCW&lt;Datasheets/radio.pdf&gt;`</v>
       </c>
       <c r="D4" t="str">
@@ -970,7 +971,7 @@
         <v>Microcontroller</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(cerebro_data!C5),"",CONCATENATE(" :download:`",cerebro_data!C5,"&lt;Datasheets/",cerebro_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D5),cerebro_data!C5,CONCATENATE(" :download:`",cerebro_data!C5,"&lt;Datasheets/",cerebro_data!D5,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`ATMEGA32U4-MUR&lt;Datasheets/MCU_32u4.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
@@ -988,7 +989,7 @@
         <v>8 MHz Resonator</v>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(cerebro_data!C6),"",CONCATENATE(" :download:`",cerebro_data!C6,"&lt;Datasheets/",cerebro_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D6),cerebro_data!C6,CONCATENATE(" :download:`",cerebro_data!C6,"&lt;Datasheets/",cerebro_data!D6,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`CSTCE8M00G55-R0&lt;Datasheets/resonator_8mhz.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
@@ -1006,7 +1007,7 @@
         <v>Fuel Gauge</v>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(cerebro_data!C7),"",CONCATENATE(" :download:`",cerebro_data!C7,"&lt;Datasheets/",cerebro_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D7),cerebro_data!C7,CONCATENATE(" :download:`",cerebro_data!C7,"&lt;Datasheets/",cerebro_data!D7,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`BQ27441DRZR-G1B&lt;Datasheets/fuel_gauge.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
@@ -1024,7 +1025,7 @@
         <v>DAC (12-Bit)</v>
       </c>
       <c r="C8" t="str">
-        <f>IF(ISBLANK(cerebro_data!C8),"",CONCATENATE(" :download:`",cerebro_data!C8,"&lt;Datasheets/",cerebro_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D8),cerebro_data!C8,CONCATENATE(" :download:`",cerebro_data!C8,"&lt;Datasheets/",cerebro_data!D8,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`LTC2630ACSC6-LZ12#TRMPBF&lt;Datasheets/DAC.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
@@ -1042,7 +1043,7 @@
         <v>Op Amp</v>
       </c>
       <c r="C9" t="str">
-        <f>IF(ISBLANK(cerebro_data!C9),"",CONCATENATE(" :download:`",cerebro_data!C9,"&lt;Datasheets/",cerebro_data!D9,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D9),cerebro_data!C9,CONCATENATE(" :download:`",cerebro_data!C9,"&lt;Datasheets/",cerebro_data!D9,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`OPA237NA/3K&lt;Datasheets/opamp.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
@@ -1060,7 +1061,7 @@
         <v>NPN Transistor</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(cerebro_data!C10),"",CONCATENATE(" :download:`",cerebro_data!C10,"&lt;Datasheets/",cerebro_data!D10,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D10),cerebro_data!C10,CONCATENATE(" :download:`",cerebro_data!C10,"&lt;Datasheets/",cerebro_data!D10,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`FJX3904TF&lt;Datasheets/npn_transistor.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
@@ -1078,7 +1079,7 @@
         <v>Boost Converter</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(ISBLANK(cerebro_data!C11),"",CONCATENATE(" :download:`",cerebro_data!C11,"&lt;Datasheets/",cerebro_data!D11,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D11),cerebro_data!C11,CONCATENATE(" :download:`",cerebro_data!C11,"&lt;Datasheets/",cerebro_data!D11,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`MIC2288YD5-TR&lt;Datasheets/boost_converter.pdf&gt;`</v>
       </c>
       <c r="D11" t="str">
@@ -1096,7 +1097,7 @@
         <v>Schottky Diode</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(ISBLANK(cerebro_data!C12),"",CONCATENATE(" :download:`",cerebro_data!C12,"&lt;Datasheets/",cerebro_data!D12,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D12),cerebro_data!C12,CONCATENATE(" :download:`",cerebro_data!C12,"&lt;Datasheets/",cerebro_data!D12,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`MBRM140T3G&lt;Datasheets/schottky.pdf&gt;`</v>
       </c>
       <c r="D12" t="str">
@@ -1114,7 +1115,7 @@
         <v>10uH Inductor</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(ISBLANK(cerebro_data!C13),"",CONCATENATE(" :download:`",cerebro_data!C13,"&lt;Datasheets/",cerebro_data!D13,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D13),cerebro_data!C13,CONCATENATE(" :download:`",cerebro_data!C13,"&lt;Datasheets/",cerebro_data!D13,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`LQH43CN100K03L&lt;Datasheets/inductor.pdf&gt;`</v>
       </c>
       <c r="D13" t="str">
@@ -1132,7 +1133,7 @@
         <v>Slide Switch</v>
       </c>
       <c r="C14" t="str">
-        <f>IF(ISBLANK(cerebro_data!C14),"",CONCATENATE(" :download:`",cerebro_data!C14,"&lt;Datasheets/",cerebro_data!D14,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D14),cerebro_data!C14,CONCATENATE(" :download:`",cerebro_data!C14,"&lt;Datasheets/",cerebro_data!D14,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
       </c>
       <c r="D14" t="str">
@@ -1150,7 +1151,7 @@
         <v>Micro USB vertical plug</v>
       </c>
       <c r="C15" t="str">
-        <f>IF(ISBLANK(cerebro_data!C15),"",CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D15),cerebro_data!C15,CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
       </c>
       <c r="D15" t="str">
@@ -1168,7 +1169,7 @@
         <v>Micro USB shielding</v>
       </c>
       <c r="C16" t="str">
-        <f>IF(ISBLANK(cerebro_data!C16),"",CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
       </c>
       <c r="D16" t="str">
@@ -1186,7 +1187,7 @@
         <v>Micro USB horizontal socket</v>
       </c>
       <c r="C17" t="str">
-        <f>IF(ISBLANK(cerebro_data!C17),"",CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D17" t="str">
@@ -1204,7 +1205,7 @@
         <v>JST-SR connector</v>
       </c>
       <c r="C18" t="str">
-        <f>IF(ISBLANK(cerebro_data!C18),"",CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`SM02B-SRSS-TB(LF)(SN)&lt;Datasheets/jst_connector.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
@@ -1222,8 +1223,8 @@
         <v>JST-SR plug with wire</v>
       </c>
       <c r="C19" t="str">
-        <f>IF(ISBLANK(cerebro_data!C19),"",CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`A02SR02SR30K152A&lt;Datasheets/&gt;`</v>
+        <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
+        <v>A02SR02SR30K152A</v>
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
@@ -1240,7 +1241,7 @@
         <v>0603 Red LED</v>
       </c>
       <c r="C20" t="str">
-        <f>IF(ISBLANK(cerebro_data!C20),"",CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
       </c>
       <c r="D20" t="str">
@@ -1258,7 +1259,7 @@
         <v>0603 Amber LED</v>
       </c>
       <c r="C21" t="str">
-        <f>IF(ISBLANK(cerebro_data!C21),"",CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
       </c>
       <c r="D21" t="str">
@@ -1937,7 +1938,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,7 +1977,7 @@
         <v>Implant PCB</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(implant_data!C2),"",CONCATENATE(" :download:`",implant_data!C2,"&lt;Datasheets/",implant_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D2),implant_data!C2,CONCATENATE(" :download:`",implant_data!C2,"&lt;Datasheets/",implant_data!D2,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`Implant 5.3&lt;Datasheets/implant_5.3.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
@@ -1994,7 +1995,7 @@
         <v>Laser Diode</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(implant_data!C3),"",CONCATENATE(" :download:`",implant_data!C3,"&lt;Datasheets/",implant_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D3),implant_data!C3,CONCATENATE(" :download:`",implant_data!C3,"&lt;Datasheets/",implant_data!D3,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`PLT5 520_B1_2_3&lt;Datasheets/green_laser_diode.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
@@ -2012,8 +2013,8 @@
         <v>Fiber</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(implant_data!C4),"",CONCATENATE(" :download:`",implant_data!C4,"&lt;Datasheets/",implant_data!D4,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`F-MBB&lt;Datasheets/&gt;`</v>
+        <f>IF(ISBLANK(implant_data!D4),implant_data!C4,CONCATENATE(" :download:`",implant_data!C4,"&lt;Datasheets/",implant_data!D4,"&gt;`"))</f>
+        <v>F-MBB</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISBLANK(implant_data!F4),"",CONCATENATE("`",implant_data!E4," &lt;",implant_data!F4,"&gt;`_"))</f>
@@ -2030,7 +2031,7 @@
         <v>UV curing adhesive</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(implant_data!C5),"",CONCATENATE(" :download:`",implant_data!C5,"&lt;Datasheets/",implant_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D5),implant_data!C5,CONCATENATE(" :download:`",implant_data!C5,"&lt;Datasheets/",implant_data!D5,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`NOA 68&lt;Datasheets/uv_adhesive.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
@@ -2048,7 +2049,7 @@
         <v>Ferrule</v>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(implant_data!C6),"",CONCATENATE(" :download:`",implant_data!C6,"&lt;Datasheets/",implant_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D6),implant_data!C6,CONCATENATE(" :download:`",implant_data!C6,"&lt;Datasheets/",implant_data!D6,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`MM-FER2007C&lt;Datasheets/ferrule.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
@@ -2066,7 +2067,7 @@
         <v>Epoxy</v>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(implant_data!C7),"",CONCATENATE(" :download:`",implant_data!C7,"&lt;Datasheets/",implant_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D7),implant_data!C7,CONCATENATE(" :download:`",implant_data!C7,"&lt;Datasheets/",implant_data!D7,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`T120023C&lt;Datasheets/epoxy.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
@@ -2084,7 +2085,7 @@
         <v>Micro USB vertical socket</v>
       </c>
       <c r="C8" t="str">
-        <f>IF(ISBLANK(implant_data!C8),"",CONCATENATE(" :download:`",implant_data!C8,"&lt;Datasheets/",implant_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!D8),implant_data!C8,CONCATENATE(" :download:`",implant_data!C8,"&lt;Datasheets/",implant_data!D8,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`1051330011&lt;Datasheets/usb_socket_vertical.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
@@ -2102,12 +2103,12 @@
         <v>0603 10 k\ |mgr|\F Capacitor</v>
       </c>
       <c r="C9" t="str">
-        <f>IF(ISBLANK(implant_data!C9),"",CONCATENATE(" :download:`",implant_data!C9,"&lt;Datasheets/",implant_data!D9,"&gt;`"))</f>
-        <v/>
+        <f>IF(ISBLANK(implant_data!D9),implant_data!C9,CONCATENATE(" :download:`",implant_data!C9,"&lt;Datasheets/",implant_data!D9,"&gt;`"))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D9" t="str">
-        <f>IF(ISBLANK(implant_data!F9),"",CONCATENATE("`",implant_data!E9," &lt;",implant_data!F9,"&gt;`_"))</f>
-        <v/>
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2120,12 +2121,12 @@
         <v>0603 20 k\ |mgr|\F Capacitor</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(implant_data!C10),"",CONCATENATE(" :download:`",implant_data!C10,"&lt;Datasheets/",implant_data!D10,"&gt;`"))</f>
-        <v/>
+        <f>IF(ISBLANK(implant_data!D10),implant_data!C10,CONCATENATE(" :download:`",implant_data!C10,"&lt;Datasheets/",implant_data!D10,"&gt;`"))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D10" t="str">
-        <f>IF(ISBLANK(implant_data!F10),"",CONCATENATE("`",implant_data!E10," &lt;",implant_data!F10,"&gt;`_"))</f>
-        <v/>
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="54" spans="2:4" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -2145,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2329,9 +2330,12 @@
       <c r="B9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="8" t="str">
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2341,10 +2345,19 @@
       <c r="B10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="8" t="str">
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="8" t="str">
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
@@ -2378,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added some pictures to "Overview" Section", updated estimated cost. Added updated "Xavier" section.
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="156">
   <si>
     <t>Qty</t>
   </si>
@@ -271,21 +271,9 @@
     <t>0603 Red LED</t>
   </si>
   <si>
-    <t>0603 10 |mgr|\F Capacitor</t>
-  </si>
-  <si>
-    <t>0603 2.2 |mgr|\F Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 8.2 |OHgr| Resistor </t>
-  </si>
-  <si>
     <t xml:space="preserve">0603 27 |OHgr| Resistor </t>
   </si>
   <si>
-    <t xml:space="preserve">0603 2 |OHgr| Resistor </t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -340,12 +328,6 @@
     <t>cerebro5.4.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">0603 6.2 k\ |OHgr| Resistor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 12 k\ |OHgr| Resistor </t>
-  </si>
-  <si>
     <t xml:space="preserve">0603 20 k\ |OHgr| Resistor </t>
   </si>
   <si>
@@ -485,6 +467,39 @@
   </si>
   <si>
     <t>voltage_translator.pdf</t>
+  </si>
+  <si>
+    <t>Qty for price</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 100 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 12 |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 2 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 4.7 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 12 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1206 0.01 |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t>10 |mgr|\H Inductor</t>
   </si>
 </sst>
 </file>
@@ -568,7 +583,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -580,7 +595,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
@@ -875,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C22" sqref="C22:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,13 +901,12 @@
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="126" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -906,8 +919,17 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <f>cerebro_data!A2</f>
         <v>1</v>
@@ -924,8 +946,18 @@
         <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`_"))</f>
         <v>`OSH Park &lt;https://oshpark.com/shared_projects/3LjXh0AX&gt;`_</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>4.95</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/F2*A2</f>
+        <v>1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f>cerebro_data!A3</f>
         <v>1</v>
@@ -942,8 +974,18 @@
         <f>IF(ISBLANK(cerebro_data!F3),"",CONCATENATE("`",cerebro_data!E3," &lt;",cerebro_data!F3,"&gt;`_"))</f>
         <v>`Sparkfun &lt;https://www.sparkfun.com/products/13851&gt;`_</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>4.95</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G21" si="0">E3/F3*A3</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f>cerebro_data!A4</f>
         <v>1</v>
@@ -960,8 +1002,18 @@
         <f>IF(ISBLANK(cerebro_data!F4),"",CONCATENATE("`",cerebro_data!E4," &lt;",cerebro_data!F4,"&gt;`_"))</f>
         <v>`LowPowerLab &lt;https://lowpowerlab.com/shop/product/158&gt;`_</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>5.95</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f>cerebro_data!A5</f>
         <v>1</v>
@@ -978,8 +1030,18 @@
         <f>IF(ISBLANK(cerebro_data!F5),"",CONCATENATE("`",cerebro_data!E5," &lt;",cerebro_data!F5,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=ATMEGA32U4-MURCT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>4.29</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
         <f>cerebro_data!A6</f>
         <v>1</v>
@@ -996,8 +1058,18 @@
         <f>IF(ISBLANK(cerebro_data!F6),"",CONCATENATE("`",cerebro_data!E6," &lt;",cerebro_data!F6,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-1195-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0.48</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
         <f>cerebro_data!A7</f>
         <v>1</v>
@@ -1014,8 +1086,18 @@
         <f>IF(ISBLANK(cerebro_data!F7),"",CONCATENATE("`",cerebro_data!E7," &lt;",cerebro_data!F7,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/texas-instruments/BQ27441DRZR-G1B/296-39942-1-ND/5177819&gt;`_</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>2.65</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f>cerebro_data!A8</f>
         <v>2</v>
@@ -1032,8 +1114,18 @@
         <f>IF(ISBLANK(cerebro_data!F8),"",CONCATENATE("`",cerebro_data!E8," &lt;",cerebro_data!F8,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/linear-technology/LTC2630ACSC6-LZ12-TRMPBF/LTC2630ACSC6-LZ12-TRMPBFCT-ND/1643783&gt;`_</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f>cerebro_data!A9</f>
         <v>2</v>
@@ -1050,8 +1142,18 @@
         <f>IF(ISBLANK(cerebro_data!F9),"",CONCATENATE("`",cerebro_data!E9," &lt;",cerebro_data!F9,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-26265-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1.52</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f>cerebro_data!A10</f>
         <v>2</v>
@@ -1068,8 +1170,18 @@
         <f>IF(ISBLANK(cerebro_data!F10),"",CONCATENATE("`",cerebro_data!E10," &lt;",cerebro_data!F10,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=FJX3904TFCT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f>cerebro_data!A11</f>
         <v>1</v>
@@ -1086,8 +1198,18 @@
         <f>IF(ISBLANK(cerebro_data!F11),"",CONCATENATE("`",cerebro_data!E11," &lt;",cerebro_data!F11,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=576-1729-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f>cerebro_data!A12</f>
         <v>1</v>
@@ -1104,8 +1226,18 @@
         <f>IF(ISBLANK(cerebro_data!F12),"",CONCATENATE("`",cerebro_data!E12," &lt;",cerebro_data!F12,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=MBRM140T3GOSCT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>0.43</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f>cerebro_data!A13</f>
         <v>1</v>
@@ -1122,8 +1254,18 @@
         <f>IF(ISBLANK(cerebro_data!F13),"",CONCATENATE("`",cerebro_data!E13," &lt;",cerebro_data!F13,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-2519-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>0.49</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f>cerebro_data!A14</f>
         <v>1</v>
@@ -1140,8 +1282,18 @@
         <f>IF(ISBLANK(cerebro_data!F14),"",CONCATENATE("`",cerebro_data!E14," &lt;",cerebro_data!F14,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f>cerebro_data!A15</f>
         <v>1</v>
@@ -1158,8 +1310,18 @@
         <f>IF(ISBLANK(cerebro_data!F15),"",CONCATENATE("`",cerebro_data!E15," &lt;",cerebro_data!F15,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f>cerebro_data!A16</f>
         <v>1</v>
@@ -1176,8 +1338,18 @@
         <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f>cerebro_data!A17</f>
         <v>1</v>
@@ -1194,8 +1366,18 @@
         <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0.46</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
         <f>cerebro_data!A18</f>
         <v>1</v>
@@ -1212,8 +1394,18 @@
         <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=455-1802-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0.44</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
         <f>cerebro_data!A19</f>
         <v>1</v>
@@ -1230,8 +1422,18 @@
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=455-3001-nd&gt;`_</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>1.08</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f>cerebro_data!A20</f>
         <v>1</v>
@@ -1248,8 +1450,18 @@
         <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <f>cerebro_data!A21</f>
         <v>1</v>
@@ -1266,137 +1478,147 @@
         <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="E21">
+        <v>0.47</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="str">
         <f>cerebro_data!A22</f>
         <v>1</v>
       </c>
       <c r="B22" t="str">
         <f>cerebro_data!B22</f>
-        <v>0603 10 |mgr|\F Capacitor</v>
+        <v>10 |mgr|\H Inductor</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" ref="C22:D26" si="0">" "</f>
+        <f t="shared" ref="C22:D30" si="1">" "</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="str">
         <f>cerebro_data!A23</f>
         <v>1</v>
       </c>
       <c r="B23" t="str">
         <f>cerebro_data!B23</f>
-        <v>0603 2.2 |mgr|\F Capacitor</v>
+        <v xml:space="preserve">1206 0.01 |OHgr| Resistor </v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="str">
         <f>cerebro_data!A24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="str">
         <f>cerebro_data!B24</f>
-        <v xml:space="preserve">0603 8.2 |OHgr| Resistor </v>
+        <v xml:space="preserve">0603 12 |OHgr| Resistor </v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="str">
         <f>cerebro_data!A25</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B25" t="str">
         <f>cerebro_data!B25</f>
         <v xml:space="preserve">0603 27 |OHgr| Resistor </v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="str">
         <f>cerebro_data!A26</f>
         <v>1</v>
       </c>
       <c r="B26" t="str">
         <f>cerebro_data!B26</f>
-        <v xml:space="preserve">0603 2 |OHgr| Resistor </v>
+        <v xml:space="preserve">0603 2 k\ |OHgr| Resistor </v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="str">
         <f>cerebro_data!A27</f>
         <v>2</v>
       </c>
-      <c r="B27" s="7" t="str">
+      <c r="B27" t="str">
         <f>cerebro_data!B27</f>
-        <v xml:space="preserve">0603 6.2 k\ |OHgr| Resistor </v>
+        <v xml:space="preserve">0603 4.7 k\ |OHgr| Resistor </v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" ref="C27:C29" si="1">" "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D27" t="str">
-        <f>" "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="str">
         <f>cerebro_data!A28</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="str">
         <f>cerebro_data!B28</f>
-        <v xml:space="preserve">0603 12 k\ |OHgr| Resistor </v>
+        <v xml:space="preserve">0805 12 k\ |OHgr| Resistor </v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D28" t="str">
-        <f>" "</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="str">
         <f>cerebro_data!A29</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29" t="str">
         <f>cerebro_data!B29</f>
@@ -1407,7 +1629,25 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D29" t="str">
-        <f>" "</f>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="str">
+        <f>cerebro_data!A30</f>
+        <v>1</v>
+      </c>
+      <c r="B30" t="str">
+        <f>cerebro_data!B30</f>
+        <v xml:space="preserve">0603 100 k\ |OHgr| Resistor </v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1425,7 +1665,7 @@
   <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,16 +1711,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1545,27 +1785,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>35</v>
@@ -1771,53 +2011,53 @@
         <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1861,68 +2101,100 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>1</v>
+      <c r="A22" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>1</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>83</v>
+      <c r="B26" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>2</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="B27" s="7" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>103</v>
+      <c r="A28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="A29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="7"/>
     </row>
     <row r="110" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F110" s="3"/>
@@ -1935,9 +2207,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1947,13 +2219,13 @@
     <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="100.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1966,8 +2238,17 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <f>cerebro_data!A2</f>
         <v>1</v>
@@ -1984,11 +2265,20 @@
         <f>IF(ISBLANK(implant_data!F2),"",CONCATENATE("`",implant_data!E2," &lt;",implant_data!F2,"&gt;`_"))</f>
         <v>`OSH Park &lt;https://oshpark.com/shared_projects/k8Ikpli6&gt;`_</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <f>cerebro_data!A3</f>
-        <v>1</v>
+      <c r="E2">
+        <v>2.1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/F2*A2</f>
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>implant_data!B3</f>
@@ -2002,8 +2292,18 @@
         <f>IF(ISBLANK(implant_data!F3),"",CONCATENATE("`",implant_data!E3," &lt;",implant_data!F3,"&gt;`_"))</f>
         <v>`World Star Tech &lt;http://www.worldstartech.com/products/laser-diodes/green-laser-diode-osram/&gt;`_</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="0">E3/F3*A3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f>cerebro_data!A4</f>
         <v>1</v>
@@ -2020,8 +2320,18 @@
         <f>IF(ISBLANK(implant_data!F4),"",CONCATENATE("`",implant_data!E4," &lt;",implant_data!F4,"&gt;`_"))</f>
         <v>`Newport &lt;https://www.newport.com/p/F-MBB&gt;`_</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2.8</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f>cerebro_data!A5</f>
         <v>1</v>
@@ -2038,8 +2348,18 @@
         <f>IF(ISBLANK(implant_data!F5),"",CONCATENATE("`",implant_data!E5," &lt;",implant_data!F5,"&gt;`_"))</f>
         <v>`Norland Products &lt;https://www.norlandproducts2.com/adhesives/adproductsdetail_header_removed.asp?Prdid=68&gt;`_</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
         <f>cerebro_data!A6</f>
         <v>1</v>
@@ -2056,8 +2376,18 @@
         <f>IF(ISBLANK(implant_data!F6),"",CONCATENATE("`",implant_data!E6," &lt;",implant_data!F6,"&gt;`_"))</f>
         <v>`Precision Fiber Products &lt;https://precisionfiberproducts.com/pfp-lc-1-25mm-od-multimode-ceramic-zirconia-ferrules/&gt;`_</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>413</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
         <f>cerebro_data!A7</f>
         <v>1</v>
@@ -2074,8 +2404,18 @@
         <f>IF(ISBLANK(implant_data!F7),"",CONCATENATE("`",implant_data!E7," &lt;",implant_data!F7,"&gt;`_"))</f>
         <v>`Fiber Instrument Sales &lt;http://www.fiberinstrumentsales.com/fis-room-cure-epoxy-2-grams.html&gt;`_</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>2.95</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f>cerebro_data!A8</f>
         <v>2</v>
@@ -2092,8 +2432,18 @@
         <f>IF(ISBLANK(implant_data!F8),"",CONCATENATE("`",implant_data!E8," &lt;",implant_data!F8,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM10134CT-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>1.06</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f>cerebro_data!A9</f>
         <v>2</v>
@@ -2111,7 +2461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f>cerebro_data!A10</f>
         <v>2</v>
@@ -2146,8 +2496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2187,131 +2537,131 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
@@ -2320,41 +2670,41 @@
         <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="8" t="str">
+        <v>122</v>
+      </c>
+      <c r="C9" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="8" t="str">
+        <v>123</v>
+      </c>
+      <c r="C10" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="8" t="str">
+      <c r="C12" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -2389,10 +2739,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2400,14 +2750,14 @@
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2420,8 +2770,17 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
         <f>base_data!A2</f>
         <v>1</v>
@@ -2438,8 +2797,18 @@
         <f>IF(ISBLANK(base_data!F2),"",CONCATENATE("`",base_data!E2," &lt;",base_data!F2,"&gt;`_"))</f>
         <v>`OSH Park &lt;https://oshpark.com/shared_projects/1H29l6K0&gt;`_</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>7.3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/F2*A2</f>
+        <v>2.4333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
         <f>base_data!A3</f>
         <v>1</v>
@@ -2456,8 +2825,18 @@
         <f>IF(ISBLANK(base_data!F3),"",CONCATENATE("`",base_data!E3," &lt;",base_data!F3,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1528-1663-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>24.95</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G5" si="0">E3/F3*A3</f>
+        <v>24.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
         <f>base_data!A4</f>
         <v>1</v>
@@ -2474,8 +2853,18 @@
         <f>IF(ISBLANK(base_data!F4),"",CONCATENATE("`",base_data!E4," &lt;",base_data!F4,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09CY7C65213-28PVXI-ND&gt;`_</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>3.44</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
         <f>base_data!A5</f>
         <v>1</v>
@@ -2492,58 +2881,68 @@
         <f>IF(ISBLANK(base_data!F5),"",CONCATENATE("`",base_data!E5," &lt;",base_data!F5,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-21929-1-nd&gt;`_</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1.32</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2617,82 +3016,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
BOM update. replaced jst-sr connector with molex microclasp. Updated Cerebro PCB from 5.4 to 5.6
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -301,45 +301,15 @@
     <t>CSTCE8M00G55-R0</t>
   </si>
   <si>
-    <t>JST-SR connector</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=455-1802-1-ND</t>
-  </si>
-  <si>
-    <t>SM02B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>A02SR02SR30K152A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=455-3001-nd</t>
-  </si>
-  <si>
-    <t>JST-SR plug with wire</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=609-4618-1-ND</t>
   </si>
   <si>
-    <t>jst_connector.pdf</t>
-  </si>
-  <si>
     <t>usb_plug_horizontal.pdf</t>
   </si>
   <si>
     <t>10118194-0001LF</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/3LjXh0AX</t>
-  </si>
-  <si>
-    <t>Cerebro 5.4</t>
-  </si>
-  <si>
-    <t>cerebro5.4.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">0603 6.2 k\ |OHgr| Resistor </t>
   </si>
   <si>
@@ -494,6 +464,36 @@
   </si>
   <si>
     <t xml:space="preserve">0603 10 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t>Cerebro 5.6</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/projects/sPd5KOMe</t>
+  </si>
+  <si>
+    <t>cerebro5.6.pdf</t>
+  </si>
+  <si>
+    <t>microclasp.pdf</t>
+  </si>
+  <si>
+    <t>Molex MicroClasp socket</t>
+  </si>
+  <si>
+    <t>Molex MicroClasp plug with wire</t>
+  </si>
+  <si>
+    <t>0559350230</t>
+  </si>
+  <si>
+    <t>0151360206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=wm16380-nd</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=wm12296-nd</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,11 +930,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Cerebro 5.4&lt;Datasheets/cerebro5.4.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`Cerebro 5.6&lt;Datasheets/cerebro5.6.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/3LjXh0AX&gt;`_</v>
+        <v>`OSH Park &lt;https://oshpark.com/projects/sPd5KOMe&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1214,15 +1214,15 @@
       </c>
       <c r="B18" t="str">
         <f>cerebro_data!B18</f>
-        <v>JST-SR connector</v>
+        <v>Molex MicroClasp socket</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`SM02B-SRSS-TB(LF)(SN)&lt;Datasheets/jst_connector.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
         <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=455-1802-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1232,15 +1232,15 @@
       </c>
       <c r="B19" t="str">
         <f>cerebro_data!B19</f>
-        <v>JST-SR plug with wire</v>
+        <v>Molex MicroClasp plug with wire</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
-        <v>A02SR02SR30K152A</v>
+        <v>0151360206</v>
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=455-3001-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1436,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1483,16 +1483,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1783,16 +1783,16 @@
         <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1800,19 +1800,19 @@
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,16 +1820,16 @@
         <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" spans="6:6" x14ac:dyDescent="0.2">
@@ -1949,7 +1949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -2223,36 +2223,36 @@
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2263,14 +2263,14 @@
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2278,39 +2278,39 @@
         <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2321,16 +2321,16 @@
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2338,10 +2338,10 @@
         <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
@@ -2350,7 +2350,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2358,27 +2358,27 @@
         <v>84</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C10" s="8" t="str">
         <f>" "</f>
@@ -2390,10 +2390,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C11" s="8" t="str">
         <f>" "</f>
@@ -2670,19 +2670,19 @@
         <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2690,19 +2690,19 @@
         <v>84</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2710,19 +2710,19 @@
         <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,19 +2730,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated Base Station BOM. Fixed some typos
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
   <si>
     <t>Qty</t>
   </si>
@@ -418,15 +418,6 @@
     <t>Base Station PCB</t>
   </si>
   <si>
-    <t>Base Station 2.1</t>
-  </si>
-  <si>
-    <t>base_station_2.1.pdf</t>
-  </si>
-  <si>
-    <t>https://oshpark.com/shared_projects/1H29l6K0</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=%09CY7C65213-28PVXI-ND</t>
   </si>
   <si>
@@ -494,6 +485,15 @@
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=wm12296-nd</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/Ed6Ntbb1</t>
+  </si>
+  <si>
+    <t>Base Station 2.2</t>
+  </si>
+  <si>
+    <t>base_station_2.2.pdf</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1436,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1483,16 +1483,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1800,19 +1800,19 @@
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,16 +1820,16 @@
         <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2358,19 +2358,19 @@
         <v>84</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2378,7 +2378,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C10" s="8" t="str">
         <f>" "</f>
@@ -2439,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2482,11 +2482,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(base_data!C2),"",CONCATENATE(" :download:`",base_data!C2,"&lt;Datasheets/",base_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Base Station 2.1&lt;Datasheets/base_station_2.1.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`Base Station 2.2&lt;Datasheets/base_station_2.2.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(base_data!F2),"",CONCATENATE("`",base_data!E2," &lt;",base_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/1H29l6K0&gt;`_</v>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/Ed6Ntbb1&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2544,14 +2544,40 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2">
+        <f>base_data!A6</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>base_data!B6</f>
+        <v>Micro USB horizontal socket</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(ISBLANK(base_data!C6),"",CONCATENATE(" :download:`",base_data!C6,"&lt;Datasheets/",base_data!D6,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(ISBLANK(base_data!F6),"",CONCATENATE("`",base_data!E6," &lt;",base_data!F6,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="2" t="str">
+        <f>base_data!A7</f>
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>base_data!B7</f>
+        <v xml:space="preserve">0603 10 k\ |OHgr| Resistor </v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(ISBLANK(base_data!C7),"",CONCATENATE(" :download:`",base_data!C7,"&lt;Datasheets/",base_data!D7,"&gt;`"))</f>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(ISBLANK(base_data!F7),"",CONCATENATE("`",base_data!E7," &lt;",base_data!F7,"&gt;`_"))</f>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
@@ -2603,18 +2629,13 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="53" spans="2:4" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D62" s="1"/>
+    <row r="52" spans="2:4" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2624,17 +2645,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -2673,16 +2694,16 @@
         <v>127</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2710,19 +2731,19 @@
         <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,32 +2751,48 @@
         <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -2785,12 +2822,17 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="E14" s="4"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2805,8 +2847,11 @@
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="4"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F110" s="3"/>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F111" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update table generator script
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2441,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Minor Xavier update. Docs should now have latest Deployment.zip
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2441,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added charging dock documentation
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088DD079-5196-0C43-A857-36BFD832E881}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,10 @@
     <sheet name="implant_data" sheetId="6" r:id="rId4"/>
     <sheet name="base" sheetId="7" r:id="rId5"/>
     <sheet name="base_data" sheetId="8" r:id="rId6"/>
+    <sheet name="dock" sheetId="9" r:id="rId7"/>
+    <sheet name="dock_data" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="181">
   <si>
     <t>Qty</t>
   </si>
@@ -494,6 +497,87 @@
   </si>
   <si>
     <t>base_station_2.2.pdf</t>
+  </si>
+  <si>
+    <t>Charging Dock PCB</t>
+  </si>
+  <si>
+    <t>Charging Dock 2.0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=%09MCP73831T-2ACI%2FOTCT-ND</t>
+  </si>
+  <si>
+    <t>lipo_charger.pdf</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT</t>
+  </si>
+  <si>
+    <t>Lipoly Charging IC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=cp-037a-nd</t>
+  </si>
+  <si>
+    <t>PJ-037A</t>
+  </si>
+  <si>
+    <t>DC Barrel Power Jack</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cui-inc/SWI12-5-N-P5R/102-3425-ND/5287234</t>
+  </si>
+  <si>
+    <t>SWI12-5-N-P5R</t>
+  </si>
+  <si>
+    <t>power_jack.pdf</t>
+  </si>
+  <si>
+    <t>power_supply.pdf</t>
+  </si>
+  <si>
+    <t>5V 2.5A Power Supply</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>0805 10 |mgr|\F Capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=732-5008-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=732-5006-ND</t>
+  </si>
+  <si>
+    <t>led_3mm_red.pdf</t>
+  </si>
+  <si>
+    <t>led_3mm_green.pdf</t>
+  </si>
+  <si>
+    <t>151031SS06000</t>
+  </si>
+  <si>
+    <t>151031VS06000</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 470 \ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 2.5 K\ |OHgr| Resistor </t>
   </si>
 </sst>
 </file>
@@ -577,7 +661,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -591,6 +675,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -889,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1437,7 +1524,7 @@
   <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1950,7 +2037,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,7 +2264,7 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2442,7 +2529,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2648,7 +2735,7 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2856,4 +2943,485 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC32778-A014-934E-B9C7-1735DC2E5111}">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="str">
+        <f>TEXT(dock_data!A2,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>dock_data!B2</f>
+        <v>Charging Dock PCB</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F2),"",CONCATENATE("`",dock_data!E2," &lt;",dock_data!F2,"&gt;`_"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="str">
+        <f>TEXT(dock_data!A3,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>dock_data!B3</f>
+        <v>Molex MicroClasp socket</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C3),"",CONCATENATE(" :download:`",dock_data!C3,"&lt;Datasheets/",dock_data!D3,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F3),"",CONCATENATE("`",dock_data!E3," &lt;",dock_data!F3,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="str">
+        <f>TEXT(dock_data!A4,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>dock_data!B4</f>
+        <v>Lipoly Charging IC</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C4),"",CONCATENATE(" :download:`",dock_data!C4,"&lt;Datasheets/",dock_data!D4,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`MCP73831T-2ACI/OT&lt;Datasheets/lipo_charger.pdf&gt;`</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F4),"",CONCATENATE("`",dock_data!E4," &lt;",dock_data!F4,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09MCP73831T-2ACI%2FOTCT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="str">
+        <f>TEXT(dock_data!A5,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>dock_data!B5</f>
+        <v>DC Barrel Power Jack</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C5),"",CONCATENATE(" :download:`",dock_data!C5,"&lt;Datasheets/",dock_data!D5,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`PJ-037A&lt;Datasheets/power_jack.pdf&gt;`</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F5),"",CONCATENATE("`",dock_data!E5," &lt;",dock_data!F5,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=cp-037a-nd&gt;`_</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="str">
+        <f>TEXT(dock_data!A6,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>dock_data!B6</f>
+        <v>5V 2.5A Power Supply</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C6),"",CONCATENATE(" :download:`",dock_data!C6,"&lt;Datasheets/",dock_data!D6,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`SWI12-5-N-P5R&lt;Datasheets/power_supply.pdf&gt;`</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F6),"",CONCATENATE("`",dock_data!E6," &lt;",dock_data!F6,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/cui-inc/SWI12-5-N-P5R/102-3425-ND/5287234&gt;`_</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="str">
+        <f>TEXT(dock_data!A7,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>dock_data!B7</f>
+        <v>Green LED</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C7),"",CONCATENATE(" :download:`",dock_data!C7,"&lt;Datasheets/",dock_data!D7,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`151031VS06000&lt;Datasheets/led_3mm_green.pdf&gt;`</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F7),"",CONCATENATE("`",dock_data!E7," &lt;",dock_data!F7,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5008-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="str">
+        <f>TEXT(dock_data!A8,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>dock_data!B8</f>
+        <v>Red LED</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C8),"",CONCATENATE(" :download:`",dock_data!C8,"&lt;Datasheets/",dock_data!D8,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`151031SS06000&lt;Datasheets/led_3mm_red.pdf&gt;`</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F8),"",CONCATENATE("`",dock_data!E8," &lt;",dock_data!F8,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5006-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="str">
+        <f>TEXT(dock_data!A9,"0")</f>
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>dock_data!B9</f>
+        <v xml:space="preserve">0805 470 \ |OHgr| Resistor </v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C9),"",CONCATENATE(" :download:`",dock_data!C9,"&lt;Datasheets/",dock_data!D9,"&gt;`"))</f>
+        <v/>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F9),"",CONCATENATE("`",dock_data!E9," &lt;",dock_data!F9,"&gt;`_"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="str">
+        <f>TEXT(dock_data!A10,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>dock_data!B10</f>
+        <v xml:space="preserve">0805 2.5 K\ |OHgr| Resistor </v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C10),"",CONCATENATE(" :download:`",dock_data!C10,"&lt;Datasheets/",dock_data!D10,"&gt;`"))</f>
+        <v/>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F10),"",CONCATENATE("`",dock_data!E10," &lt;",dock_data!F10,"&gt;`_"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="str">
+        <f>TEXT(dock_data!A11,"0")</f>
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>dock_data!B11</f>
+        <v>0805 10 |mgr|\F Capacitor</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!C11),"",CONCATENATE(" :download:`",dock_data!C11,"&lt;Datasheets/",dock_data!D11,"&gt;`"))</f>
+        <v/>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>IF(ISBLANK(dock_data!F11),"",CONCATENATE("`",dock_data!E11," &lt;",dock_data!F11,"&gt;`_"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="4:4" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15D8D56-C8BD-6843-8F65-27683E07D936}">
+  <dimension ref="A1:F113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F113" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added pogo connector resources. Added instructions for burning bootloader onto Cerebro
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088DD079-5196-0C43-A857-36BFD832E881}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4083404C-6656-CE43-AB95-FD5AEA90210B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="base_data" sheetId="8" r:id="rId6"/>
     <sheet name="dock" sheetId="9" r:id="rId7"/>
     <sheet name="dock_data" sheetId="10" r:id="rId8"/>
+    <sheet name="progammer" sheetId="11" r:id="rId9"/>
+    <sheet name="programmer_data" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="232">
   <si>
     <t>Qty</t>
   </si>
@@ -172,9 +174,6 @@
     <t>https://www.digikey.com/products/en?keywords=160-1447-1-ND</t>
   </si>
   <si>
-    <t>0603 Amber LED</t>
-  </si>
-  <si>
     <t>led_amber.pdf</t>
   </si>
   <si>
@@ -271,24 +270,6 @@
     <t>battery_400mah.pdf</t>
   </si>
   <si>
-    <t>0603 Red LED</t>
-  </si>
-  <si>
-    <t>0603 10 |mgr|\F Capacitor</t>
-  </si>
-  <si>
-    <t>0603 2.2 |mgr|\F Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 8.2 |OHgr| Resistor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 27 |OHgr| Resistor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 2 |OHgr| Resistor </t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -313,12 +294,6 @@
     <t>10118194-0001LF</t>
   </si>
   <si>
-    <t xml:space="preserve">0603 6.2 k\ |OHgr| Resistor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603 12 k\ |OHgr| Resistor </t>
-  </si>
-  <si>
     <t xml:space="preserve">0603 20 k\ |OHgr| Resistor </t>
   </si>
   <si>
@@ -578,6 +553,186 @@
   </si>
   <si>
     <t xml:space="preserve">0805 2.5 K\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=%09AP2112K-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>AP2112K-3.3TRG1</t>
+  </si>
+  <si>
+    <t>3.3V Linear Regulator</t>
+  </si>
+  <si>
+    <t>regulator_3v_linear.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=P0.01BVCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=541-27.0SCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1276-1066-1-nd</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=587-1286-1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=P12.00BYCT-ND</t>
+  </si>
+  <si>
+    <t>Red LED (0603)</t>
+  </si>
+  <si>
+    <t>Amber LED (0603)</t>
+  </si>
+  <si>
+    <t>470 nF Capacitor (0805)</t>
+  </si>
+  <si>
+    <t>1 |mgr|\F Capacitor (0805)</t>
+  </si>
+  <si>
+    <t>2.2 |mgr|\F Capacitor (0805)</t>
+  </si>
+  <si>
+    <t>10 |mgr|\F Capacitor (0805)</t>
+  </si>
+  <si>
+    <t>0.01 |OHgr| Resistor (1206)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 |OHgr| Resistor (0603) </t>
+  </si>
+  <si>
+    <t>27 |OHgr| Resistor (0603)</t>
+  </si>
+  <si>
+    <t>2 k\ |OHgr| Resistor (0603)</t>
+  </si>
+  <si>
+    <t>4.7 k\ |OHgr| Resistor (0603)</t>
+  </si>
+  <si>
+    <t>12 k\ |OHgr| Resistor (0805)</t>
+  </si>
+  <si>
+    <t>20 k\ |OHgr| Resistor (0603)</t>
+  </si>
+  <si>
+    <t>100 k\ |OHgr| Resistor (0603)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND</t>
+  </si>
+  <si>
+    <t>Programmer PCB</t>
+  </si>
+  <si>
+    <t>Cerebro ICSP 1.2</t>
+  </si>
+  <si>
+    <t>6 Pin Socket</t>
+  </si>
+  <si>
+    <t>75869-331LF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=609-5122-ND</t>
+  </si>
+  <si>
+    <t>ICSP_socket.pdf</t>
+  </si>
+  <si>
+    <t>Spear Head Pogo Pin</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>92492A717</t>
+  </si>
+  <si>
+    <t>M3 x 0.5 Screw</t>
+  </si>
+  <si>
+    <t>M3 Nut</t>
+  </si>
+  <si>
+    <t>90695A033</t>
+  </si>
+  <si>
+    <t>93657A203</t>
+  </si>
+  <si>
+    <t>Nylon Spacer</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#93657A203</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#92492A717</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#90695A033</t>
+  </si>
+  <si>
+    <t>m3_nylon_screw.pdf</t>
+  </si>
+  <si>
+    <t>nylon_spacer.pdf</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2430</t>
+  </si>
+  <si>
+    <t>2430</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/394</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>394</t>
+  </si>
+  <si>
+    <t>m3_nut.pdf</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/PXMM4F8R</t>
+  </si>
+  <si>
+    <t>Needle Head Pogo Pin</t>
   </si>
 </sst>
 </file>
@@ -661,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -673,7 +828,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -977,7 +1131,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,33 +1257,33 @@
       </c>
       <c r="B7" t="str">
         <f>cerebro_data!B7</f>
-        <v>Fuel Gauge</v>
+        <v>3.3V Linear Regulator</v>
       </c>
       <c r="C7" t="str">
         <f>IF(ISBLANK(cerebro_data!D7),cerebro_data!C7,CONCATENATE(" :download:`",cerebro_data!C7,"&lt;Datasheets/",cerebro_data!D7,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`BQ27441DRZR-G1B&lt;Datasheets/fuel_gauge.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`AP2112K-3.3TRG1&lt;Datasheets/regulator_3v_linear.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISBLANK(cerebro_data!F7),"",CONCATENATE("`",cerebro_data!E7," &lt;",cerebro_data!F7,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/texas-instruments/BQ27441DRZR-G1B/296-39942-1-ND/5177819&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09AP2112K-3.3TRG1DICT-ND&gt;`_</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="2" t="str">
         <f>cerebro_data!A8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="str">
         <f>cerebro_data!B8</f>
-        <v>DAC (12-Bit)</v>
+        <v>Fuel Gauge</v>
       </c>
       <c r="C8" t="str">
         <f>IF(ISBLANK(cerebro_data!D8),cerebro_data!C8,CONCATENATE(" :download:`",cerebro_data!C8,"&lt;Datasheets/",cerebro_data!D8,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LTC2630ACSC6-LZ12#TRMPBF&lt;Datasheets/DAC.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`BQ27441DRZR-G1B&lt;Datasheets/fuel_gauge.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(cerebro_data!F8),"",CONCATENATE("`",cerebro_data!E8," &lt;",cerebro_data!F8,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/linear-technology/LTC2630ACSC6-LZ12-TRMPBF/LTC2630ACSC6-LZ12-TRMPBFCT-ND/1643783&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/texas-instruments/BQ27441DRZR-G1B/296-39942-1-ND/5177819&gt;`_</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1139,15 +1293,15 @@
       </c>
       <c r="B9" t="str">
         <f>cerebro_data!B9</f>
-        <v>Op Amp</v>
+        <v>DAC (12-Bit)</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(cerebro_data!D9),cerebro_data!C9,CONCATENATE(" :download:`",cerebro_data!C9,"&lt;Datasheets/",cerebro_data!D9,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`OPA237NA/3K&lt;Datasheets/opamp.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`LTC2630ACSC6-LZ12#TRMPBF&lt;Datasheets/DAC.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(cerebro_data!F9),"",CONCATENATE("`",cerebro_data!E9," &lt;",cerebro_data!F9,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-26265-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/linear-technology/LTC2630ACSC6-LZ12-TRMPBF/LTC2630ACSC6-LZ12-TRMPBFCT-ND/1643783&gt;`_</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1157,33 +1311,33 @@
       </c>
       <c r="B10" t="str">
         <f>cerebro_data!B10</f>
-        <v>NPN Transistor</v>
+        <v>Op Amp</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(cerebro_data!D10),cerebro_data!C10,CONCATENATE(" :download:`",cerebro_data!C10,"&lt;Datasheets/",cerebro_data!D10,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`FJX3904TF&lt;Datasheets/npn_transistor.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`OPA237NA/3K&lt;Datasheets/opamp.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(cerebro_data!F10),"",CONCATENATE("`",cerebro_data!E10," &lt;",cerebro_data!F10,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=FJX3904TFCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-26265-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f>cerebro_data!A11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="str">
         <f>cerebro_data!B11</f>
-        <v>Boost Converter</v>
+        <v>NPN Transistor</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(cerebro_data!D11),cerebro_data!C11,CONCATENATE(" :download:`",cerebro_data!C11,"&lt;Datasheets/",cerebro_data!D11,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`MIC2288YD5-TR&lt;Datasheets/boost_converter.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`FJX3904TF&lt;Datasheets/npn_transistor.pdf&gt;`</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(cerebro_data!F11),"",CONCATENATE("`",cerebro_data!E11," &lt;",cerebro_data!F11,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=576-1729-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=FJX3904TFCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1193,15 +1347,15 @@
       </c>
       <c r="B12" t="str">
         <f>cerebro_data!B12</f>
-        <v>Schottky Diode</v>
+        <v>Boost Converter</v>
       </c>
       <c r="C12" t="str">
         <f>IF(ISBLANK(cerebro_data!D12),cerebro_data!C12,CONCATENATE(" :download:`",cerebro_data!C12,"&lt;Datasheets/",cerebro_data!D12,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`MBRM140T3G&lt;Datasheets/schottky.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`MIC2288YD5-TR&lt;Datasheets/boost_converter.pdf&gt;`</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISBLANK(cerebro_data!F12),"",CONCATENATE("`",cerebro_data!E12," &lt;",cerebro_data!F12,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=MBRM140T3GOSCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=576-1729-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1211,15 +1365,15 @@
       </c>
       <c r="B13" t="str">
         <f>cerebro_data!B13</f>
-        <v>10uH Inductor</v>
+        <v>Schottky Diode</v>
       </c>
       <c r="C13" t="str">
         <f>IF(ISBLANK(cerebro_data!D13),cerebro_data!C13,CONCATENATE(" :download:`",cerebro_data!C13,"&lt;Datasheets/",cerebro_data!D13,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LQH43CN100K03L&lt;Datasheets/inductor.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`MBRM140T3G&lt;Datasheets/schottky.pdf&gt;`</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISBLANK(cerebro_data!F13),"",CONCATENATE("`",cerebro_data!E13," &lt;",cerebro_data!F13,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-2519-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=MBRM140T3GOSCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1229,15 +1383,15 @@
       </c>
       <c r="B14" t="str">
         <f>cerebro_data!B14</f>
-        <v>Slide Switch</v>
+        <v>10uH Inductor</v>
       </c>
       <c r="C14" t="str">
         <f>IF(ISBLANK(cerebro_data!D14),cerebro_data!C14,CONCATENATE(" :download:`",cerebro_data!C14,"&lt;Datasheets/",cerebro_data!D14,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`LQH43CN100K03L&lt;Datasheets/inductor.pdf&gt;`</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISBLANK(cerebro_data!F14),"",CONCATENATE("`",cerebro_data!E14," &lt;",cerebro_data!F14,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-2519-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1247,15 +1401,15 @@
       </c>
       <c r="B15" t="str">
         <f>cerebro_data!B15</f>
-        <v>Micro USB vertical plug</v>
+        <v>Slide Switch</v>
       </c>
       <c r="C15" t="str">
         <f>IF(ISBLANK(cerebro_data!D15),cerebro_data!C15,CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK(cerebro_data!F15),"",CONCATENATE("`",cerebro_data!E15," &lt;",cerebro_data!F15,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,15 +1419,15 @@
       </c>
       <c r="B16" t="str">
         <f>cerebro_data!B16</f>
-        <v>Micro USB shielding</v>
+        <v>Micro USB vertical plug</v>
       </c>
       <c r="C16" t="str">
         <f>IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
       </c>
       <c r="D16" t="str">
         <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,33 +1437,33 @@
       </c>
       <c r="B17" t="str">
         <f>cerebro_data!B17</f>
-        <v>Micro USB horizontal socket</v>
+        <v>Micro USB shielding</v>
       </c>
       <c r="C17" t="str">
         <f>IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="str">
+      <c r="A18" s="2">
         <f>cerebro_data!A18</f>
         <v>1</v>
       </c>
       <c r="B18" t="str">
         <f>cerebro_data!B18</f>
-        <v>Molex MicroClasp socket</v>
+        <v>Micro USB horizontal socket</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
         <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1319,33 +1473,33 @@
       </c>
       <c r="B19" t="str">
         <f>cerebro_data!B19</f>
-        <v>Molex MicroClasp plug with wire</v>
+        <v>Molex MicroClasp socket</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
-        <v>0151360206</v>
+        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="2" t="str">
         <f>cerebro_data!A20</f>
         <v>1</v>
       </c>
       <c r="B20" t="str">
         <f>cerebro_data!B20</f>
-        <v>0603 Red LED</v>
+        <v>Molex MicroClasp plug with wire</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
+        <v>0151360206</v>
       </c>
       <c r="D20" t="str">
         <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1355,15 +1509,15 @@
       </c>
       <c r="B21" t="str">
         <f>cerebro_data!B21</f>
-        <v>0603 Amber LED</v>
+        <v>Red LED (0603)</v>
       </c>
       <c r="C21" t="str">
         <f>IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
       </c>
       <c r="D21" t="str">
         <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1373,51 +1527,51 @@
       </c>
       <c r="B22" t="str">
         <f>cerebro_data!B22</f>
-        <v>0603 10 |mgr|\F Capacitor</v>
+        <v>Amber LED (0603)</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" ref="C22:D26" si="0">" "</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!D22),cerebro_data!C22,CONCATENATE(" :download:`",cerebro_data!C22,"&lt;Datasheets/",cerebro_data!D22,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F22),"",CONCATENATE("`",cerebro_data!E22," &lt;",cerebro_data!F22,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="2" t="str">
         <f>cerebro_data!A23</f>
         <v>1</v>
       </c>
       <c r="B23" t="str">
         <f>cerebro_data!B23</f>
-        <v>0603 2.2 |mgr|\F Capacitor</v>
+        <v>470 nF Capacitor (0805)</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F23),"",CONCATENATE("`",cerebro_data!E23," &lt;",cerebro_data!F23,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="2" t="str">
         <f>cerebro_data!A24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="str">
         <f>cerebro_data!B24</f>
-        <v xml:space="preserve">0603 8.2 |OHgr| Resistor </v>
+        <v>1 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F24),"",CONCATENATE("`",cerebro_data!E24," &lt;",cerebro_data!F24,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1427,92 +1581,409 @@
       </c>
       <c r="B25" t="str">
         <f>cerebro_data!B25</f>
-        <v xml:space="preserve">0603 27 |OHgr| Resistor </v>
+        <v>2.2 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F25),"",CONCATENATE("`",cerebro_data!E25," &lt;",cerebro_data!F25,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="2" t="str">
         <f>cerebro_data!A26</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" t="str">
         <f>cerebro_data!B26</f>
-        <v xml:space="preserve">0603 2 |OHgr| Resistor </v>
+        <v>10 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F26),"",CONCATENATE("`",cerebro_data!E26," &lt;",cerebro_data!F26,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="2" t="str">
         <f>cerebro_data!A27</f>
-        <v>2</v>
-      </c>
-      <c r="B27" s="7" t="str">
+        <v>1</v>
+      </c>
+      <c r="B27" t="str">
         <f>cerebro_data!B27</f>
-        <v xml:space="preserve">0603 6.2 k\ |OHgr| Resistor </v>
+        <v>0.01 |OHgr| Resistor (1206)</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" ref="C27:C29" si="1">" "</f>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D27" t="str">
-        <f>" "</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F27),"",CONCATENATE("`",cerebro_data!E27," &lt;",cerebro_data!F27,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="2" t="str">
         <f>cerebro_data!A28</f>
         <v>2</v>
       </c>
       <c r="B28" t="str">
         <f>cerebro_data!B28</f>
-        <v xml:space="preserve">0603 12 k\ |OHgr| Resistor </v>
+        <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D28" t="str">
-        <f>" "</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F28),"",CONCATENATE("`",cerebro_data!E28," &lt;",cerebro_data!F28,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="2" t="str">
         <f>cerebro_data!A29</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29" t="str">
         <f>cerebro_data!B29</f>
-        <v xml:space="preserve">0603 20 k\ |OHgr| Resistor </v>
+        <v>27 |OHgr| Resistor (0603)</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="D29" t="str">
-        <f>" "</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK(cerebro_data!F29),"",CONCATENATE("`",cerebro_data!E29," &lt;",cerebro_data!F29,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <f>cerebro_data!A30</f>
+        <v>1</v>
+      </c>
+      <c r="B30" t="str">
+        <f>cerebro_data!B30</f>
+        <v>2 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C30" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(ISBLANK(cerebro_data!F30),"",CONCATENATE("`",cerebro_data!E30," &lt;",cerebro_data!F30,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="str">
+        <f>cerebro_data!A31</f>
+        <v>2</v>
+      </c>
+      <c r="B31" t="str">
+        <f>cerebro_data!B31</f>
+        <v>4.7 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C31" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <f>IF(ISBLANK(cerebro_data!F31),"",CONCATENATE("`",cerebro_data!E31," &lt;",cerebro_data!F31,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f>cerebro_data!A32</f>
+        <v>2</v>
+      </c>
+      <c r="B32" t="str">
+        <f>cerebro_data!B32</f>
+        <v>12 k\ |OHgr| Resistor (0805)</v>
+      </c>
+      <c r="C32" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <f>IF(ISBLANK(cerebro_data!F32),"",CONCATENATE("`",cerebro_data!E32," &lt;",cerebro_data!F32,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="str">
+        <f>cerebro_data!A33</f>
+        <v>6</v>
+      </c>
+      <c r="B33" t="str">
+        <f>cerebro_data!B33</f>
+        <v>20 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C33" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(ISBLANK(cerebro_data!F33),"",CONCATENATE("`",cerebro_data!E33," &lt;",cerebro_data!F33,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f>cerebro_data!A34</f>
+        <v>2</v>
+      </c>
+      <c r="B34" t="str">
+        <f>cerebro_data!B34</f>
+        <v>100 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C34" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <f>IF(ISBLANK(cerebro_data!F34),"",CONCATENATE("`",cerebro_data!E34," &lt;",cerebro_data!F34,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="74" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="83" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D83" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC250F28-3064-E743-B78A-8D6381A20273}">
+  <dimension ref="A1:F113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F113" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,10 +1992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,9 +2003,9 @@
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="146.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82" style="2" customWidth="1"/>
     <col min="7" max="7" width="130.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -1570,16 +2041,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1593,7 +2064,7 @@
         <v>1570</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>29</v>
@@ -1630,76 +2101,76 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1707,19 +2178,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1727,39 +2198,39 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
-        <v>49</v>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>58</v>
+      <c r="F11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1767,19 +2238,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1787,59 +2258,59 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>57</v>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>61</v>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1850,16 +2321,16 @@
         <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1870,73 +2341,73 @@
         <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>1</v>
+      <c r="A20" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1944,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>188</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>46</v>
@@ -1956,7 +2427,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1964,23 +2435,47 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>79</v>
+        <v>189</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>1</v>
+      <c r="A23" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>190</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>1</v>
+      <c r="A24" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>191</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1988,43 +2483,143 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>192</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>1</v>
+      <c r="A26" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>193</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>2</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="B32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F110" s="3"/>
+      <c r="B34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F115" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2158,7 +2753,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f>cerebro_data!A7</f>
+        <f>cerebro_data!A8</f>
         <v>1</v>
       </c>
       <c r="B7" s="2" t="str">
@@ -2176,7 +2771,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <f>cerebro_data!A8</f>
+        <f>cerebro_data!A9</f>
         <v>2</v>
       </c>
       <c r="B8" s="2" t="str">
@@ -2194,7 +2789,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f>cerebro_data!A9</f>
+        <f>cerebro_data!A10</f>
         <v>2</v>
       </c>
       <c r="B9" s="2" t="str">
@@ -2212,7 +2807,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f>cerebro_data!A10</f>
+        <f>cerebro_data!A11</f>
         <v>2</v>
       </c>
       <c r="B10" s="2" t="str">
@@ -2230,7 +2825,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <f>cerebro_data!A11</f>
+        <f>cerebro_data!A12</f>
         <v>1</v>
       </c>
       <c r="B11" s="2" t="str">
@@ -2304,131 +2899,131 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
@@ -2437,61 +3032,61 @@
         <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="8" t="str">
+        <v>131</v>
+      </c>
+      <c r="C10" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="8" t="str">
+        <v>85</v>
+      </c>
+      <c r="C11" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="8" t="str">
+      <c r="C13" s="7" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -2775,82 +3370,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2858,27 +3453,27 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2950,38 +3545,38 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="C44" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="22.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="str">
+      <c r="A2" s="7" t="str">
         <f>TEXT(dock_data!A2,"0")</f>
         <v>1</v>
       </c>
@@ -2989,13 +3584,13 @@
         <f>dock_data!B2</f>
         <v>Charging Dock PCB</v>
       </c>
-      <c r="D2" s="8" t="str">
+      <c r="D2" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F2),"",CONCATENATE("`",dock_data!E2," &lt;",dock_data!F2,"&gt;`_"))</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="str">
+      <c r="A3" s="7" t="str">
         <f>TEXT(dock_data!A3,"0")</f>
         <v>6</v>
       </c>
@@ -3003,17 +3598,17 @@
         <f>dock_data!B3</f>
         <v>Molex MicroClasp socket</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C3),"",CONCATENATE(" :download:`",dock_data!C3,"&lt;Datasheets/",dock_data!D3,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
       </c>
-      <c r="D3" s="8" t="str">
+      <c r="D3" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F3),"",CONCATENATE("`",dock_data!E3," &lt;",dock_data!F3,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="str">
+      <c r="A4" s="7" t="str">
         <f>TEXT(dock_data!A4,"0")</f>
         <v>6</v>
       </c>
@@ -3021,17 +3616,17 @@
         <f>dock_data!B4</f>
         <v>Lipoly Charging IC</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C4),"",CONCATENATE(" :download:`",dock_data!C4,"&lt;Datasheets/",dock_data!D4,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`MCP73831T-2ACI/OT&lt;Datasheets/lipo_charger.pdf&gt;`</v>
       </c>
-      <c r="D4" s="8" t="str">
+      <c r="D4" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F4),"",CONCATENATE("`",dock_data!E4," &lt;",dock_data!F4,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09MCP73831T-2ACI%2FOTCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="str">
+      <c r="A5" s="7" t="str">
         <f>TEXT(dock_data!A5,"0")</f>
         <v>1</v>
       </c>
@@ -3039,17 +3634,17 @@
         <f>dock_data!B5</f>
         <v>DC Barrel Power Jack</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C5),"",CONCATENATE(" :download:`",dock_data!C5,"&lt;Datasheets/",dock_data!D5,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`PJ-037A&lt;Datasheets/power_jack.pdf&gt;`</v>
       </c>
-      <c r="D5" s="8" t="str">
+      <c r="D5" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F5),"",CONCATENATE("`",dock_data!E5," &lt;",dock_data!F5,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=cp-037a-nd&gt;`_</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="str">
+      <c r="A6" s="7" t="str">
         <f>TEXT(dock_data!A6,"0")</f>
         <v>1</v>
       </c>
@@ -3057,17 +3652,17 @@
         <f>dock_data!B6</f>
         <v>5V 2.5A Power Supply</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C6),"",CONCATENATE(" :download:`",dock_data!C6,"&lt;Datasheets/",dock_data!D6,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`SWI12-5-N-P5R&lt;Datasheets/power_supply.pdf&gt;`</v>
       </c>
-      <c r="D6" s="8" t="str">
+      <c r="D6" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F6),"",CONCATENATE("`",dock_data!E6," &lt;",dock_data!F6,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/cui-inc/SWI12-5-N-P5R/102-3425-ND/5287234&gt;`_</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="str">
+      <c r="A7" s="7" t="str">
         <f>TEXT(dock_data!A7,"0")</f>
         <v>6</v>
       </c>
@@ -3075,17 +3670,17 @@
         <f>dock_data!B7</f>
         <v>Green LED</v>
       </c>
-      <c r="C7" s="8" t="str">
+      <c r="C7" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C7),"",CONCATENATE(" :download:`",dock_data!C7,"&lt;Datasheets/",dock_data!D7,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`151031VS06000&lt;Datasheets/led_3mm_green.pdf&gt;`</v>
       </c>
-      <c r="D7" s="8" t="str">
+      <c r="D7" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F7),"",CONCATENATE("`",dock_data!E7," &lt;",dock_data!F7,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5008-ND&gt;`_</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="7" t="str">
         <f>TEXT(dock_data!A8,"0")</f>
         <v>6</v>
       </c>
@@ -3093,17 +3688,17 @@
         <f>dock_data!B8</f>
         <v>Red LED</v>
       </c>
-      <c r="C8" s="8" t="str">
+      <c r="C8" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C8),"",CONCATENATE(" :download:`",dock_data!C8,"&lt;Datasheets/",dock_data!D8,"&gt;`"))</f>
         <v xml:space="preserve"> :download:`151031SS06000&lt;Datasheets/led_3mm_red.pdf&gt;`</v>
       </c>
-      <c r="D8" s="8" t="str">
+      <c r="D8" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F8),"",CONCATENATE("`",dock_data!E8," &lt;",dock_data!F8,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5006-ND&gt;`_</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="str">
+      <c r="A9" s="7" t="str">
         <f>TEXT(dock_data!A9,"0")</f>
         <v>12</v>
       </c>
@@ -3111,17 +3706,17 @@
         <f>dock_data!B9</f>
         <v xml:space="preserve">0805 470 \ |OHgr| Resistor </v>
       </c>
-      <c r="C9" s="8" t="str">
+      <c r="C9" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C9),"",CONCATENATE(" :download:`",dock_data!C9,"&lt;Datasheets/",dock_data!D9,"&gt;`"))</f>
         <v/>
       </c>
-      <c r="D9" s="8" t="str">
+      <c r="D9" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F9),"",CONCATENATE("`",dock_data!E9," &lt;",dock_data!F9,"&gt;`_"))</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="7" t="str">
         <f>TEXT(dock_data!A10,"0")</f>
         <v>6</v>
       </c>
@@ -3129,17 +3724,17 @@
         <f>dock_data!B10</f>
         <v xml:space="preserve">0805 2.5 K\ |OHgr| Resistor </v>
       </c>
-      <c r="C10" s="8" t="str">
+      <c r="C10" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C10),"",CONCATENATE(" :download:`",dock_data!C10,"&lt;Datasheets/",dock_data!D10,"&gt;`"))</f>
         <v/>
       </c>
-      <c r="D10" s="8" t="str">
+      <c r="D10" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F10),"",CONCATENATE("`",dock_data!E10," &lt;",dock_data!F10,"&gt;`_"))</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="str">
+      <c r="A11" s="7" t="str">
         <f>TEXT(dock_data!A11,"0")</f>
         <v>12</v>
       </c>
@@ -3147,18 +3742,18 @@
         <f>dock_data!B11</f>
         <v>0805 10 |mgr|\F Capacitor</v>
       </c>
-      <c r="C11" s="8" t="str">
+      <c r="C11" s="7" t="str">
         <f>IF(ISBLANK(dock_data!C11),"",CONCATENATE(" :download:`",dock_data!C11,"&lt;Datasheets/",dock_data!D11,"&gt;`"))</f>
         <v/>
       </c>
-      <c r="D11" s="8" t="str">
+      <c r="D11" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F11),"",CONCATENATE("`",dock_data!E11," &lt;",dock_data!F11,"&gt;`_"))</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="4:4" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" s="9"/>
+      <c r="D60" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3170,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15D8D56-C8BD-6843-8F65-27683E07D936}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F47" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,13 +3806,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
@@ -3227,62 +3822,62 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3290,67 +3885,67 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3359,10 +3954,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3371,10 +3966,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -3424,4 +4019,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3A5705-ADFD-734A-AD52-C17C677E2A49}">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="str">
+        <f>TEXT(programmer_data!A2,"0")</f>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>programmer_data!B2</f>
+        <v>Programmer PCB</v>
+      </c>
+      <c r="C2" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C2),"",CONCATENATE(" :download:`",programmer_data!C2,"&lt;Datasheets/",programmer_data!D2,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`Cerebro ICSP 1.2&lt;Datasheets/&gt;`</v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F2),"",CONCATENATE("`",programmer_data!E2," &lt;",programmer_data!F2,"&gt;`_"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/PXMM4F8R&gt;`_</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="str">
+        <f>TEXT(programmer_data!A3,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>programmer_data!B3</f>
+        <v>6 Pin Socket</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C3),"",CONCATENATE(" :download:`",programmer_data!C3,"&lt;Datasheets/",programmer_data!D3,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`75869-331LF&lt;Datasheets/ICSP_socket.pdf&gt;`</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F3),"",CONCATENATE("`",programmer_data!E3," &lt;",programmer_data!F3,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-5122-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="str">
+        <f>TEXT(programmer_data!A4,"0")</f>
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>programmer_data!B4</f>
+        <v>Spear Head Pogo Pin</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C4),"",CONCATENATE(" :download:`",programmer_data!C4,"&lt;Datasheets/",programmer_data!D4,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`394&lt;Datasheets/&gt;`</v>
+      </c>
+      <c r="D4" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F4),"",CONCATENATE("`",programmer_data!E4," &lt;",programmer_data!F4,"&gt;`_"))</f>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/394&gt;`_</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="str">
+        <f>TEXT(programmer_data!A5,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>programmer_data!B5</f>
+        <v>Needle Head Pogo Pin</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C5),"",CONCATENATE(" :download:`",programmer_data!C5,"&lt;Datasheets/",programmer_data!D5,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`2430&lt;Datasheets/&gt;`</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F5),"",CONCATENATE("`",programmer_data!E5," &lt;",programmer_data!F5,"&gt;`_"))</f>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/2430&gt;`_</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="str">
+        <f>TEXT(programmer_data!A6,"0")</f>
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>programmer_data!B6</f>
+        <v>M3 x 0.5 Screw</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C6),"",CONCATENATE(" :download:`",programmer_data!C6,"&lt;Datasheets/",programmer_data!D6,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`92492A717&lt;Datasheets/m3_nylon_screw.pdf&gt;`</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F6),"",CONCATENATE("`",programmer_data!E6," &lt;",programmer_data!F6,"&gt;`_"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#92492A717&gt;`_</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="str">
+        <f>TEXT(programmer_data!A7,"0")</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>programmer_data!B7</f>
+        <v>Nylon Spacer</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C7),"",CONCATENATE(" :download:`",programmer_data!C7,"&lt;Datasheets/",programmer_data!D7,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`93657A203&lt;Datasheets/nylon_spacer.pdf&gt;`</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F7),"",CONCATENATE("`",programmer_data!E7," &lt;",programmer_data!F7,"&gt;`_"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#93657A203&gt;`_</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="str">
+        <f>TEXT(programmer_data!A8,"0")</f>
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>programmer_data!B8</f>
+        <v>M3 Nut</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!C8),"",CONCATENATE(" :download:`",programmer_data!C8,"&lt;Datasheets/",programmer_data!D8,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`90695A033&lt;Datasheets/m3_nut.pdf&gt;`</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f>IF(ISBLANK(programmer_data!F8),"",CONCATENATE("`",programmer_data!E8," &lt;",programmer_data!F8,"&gt;`_"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#90695A033&gt;`_</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated overivew text and added pictures. Added links to USB drivers.
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4083404C-6656-CE43-AB95-FD5AEA90210B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3796FAEA-06F3-9A42-B81E-95FAE8E30298}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="238">
   <si>
     <t>Qty</t>
   </si>
@@ -435,15 +435,6 @@
     <t xml:space="preserve">0603 10 k\ |OHgr| Resistor </t>
   </si>
   <si>
-    <t>Cerebro 5.6</t>
-  </si>
-  <si>
-    <t>https://oshpark.com/projects/sPd5KOMe</t>
-  </si>
-  <si>
-    <t>cerebro5.6.pdf</t>
-  </si>
-  <si>
     <t>microclasp.pdf</t>
   </si>
   <si>
@@ -733,6 +724,33 @@
   </si>
   <si>
     <t>Needle Head Pogo Pin</t>
+  </si>
+  <si>
+    <t>2mm Pitch Male Header</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=952-1992-nd</t>
+  </si>
+  <si>
+    <t>header_male_2mm.pdf</t>
+  </si>
+  <si>
+    <t>M22-2510805</t>
+  </si>
+  <si>
+    <t>Cerebro 5.7</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/MiiC2fHG</t>
+  </si>
+  <si>
+    <t>cerebro5.7.pdf</t>
+  </si>
+  <si>
+    <t>charging_dock_2.0.pdf</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/hz6upCEq</t>
   </si>
 </sst>
 </file>
@@ -1131,13 +1149,13 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="126" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1171,11 +1189,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Cerebro 5.6&lt;Datasheets/cerebro5.6.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`Cerebro 5.7&lt;Datasheets/cerebro5.7.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/projects/sPd5KOMe&gt;`_</v>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/MiiC2fHG&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1395,21 +1413,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="2" t="str">
         <f>cerebro_data!A15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="str">
         <f>cerebro_data!B15</f>
-        <v>Slide Switch</v>
+        <v>2mm Pitch Male Header</v>
       </c>
       <c r="C15" t="str">
         <f>IF(ISBLANK(cerebro_data!D15),cerebro_data!C15,CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`M22-2510805&lt;Datasheets/header_male_2mm.pdf&gt;`</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK(cerebro_data!F15),"",CONCATENATE("`",cerebro_data!E15," &lt;",cerebro_data!F15,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=952-1992-nd&gt;`_</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,15 +1437,15 @@
       </c>
       <c r="B16" t="str">
         <f>cerebro_data!B16</f>
-        <v>Micro USB vertical plug</v>
+        <v>Slide Switch</v>
       </c>
       <c r="C16" t="str">
         <f>IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
       </c>
       <c r="D16" t="str">
         <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1437,15 +1455,15 @@
       </c>
       <c r="B17" t="str">
         <f>cerebro_data!B17</f>
-        <v>Micro USB shielding</v>
+        <v>Micro USB vertical plug</v>
       </c>
       <c r="C17" t="str">
         <f>IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1455,33 +1473,33 @@
       </c>
       <c r="B18" t="str">
         <f>cerebro_data!B18</f>
-        <v>Micro USB horizontal socket</v>
+        <v>Micro USB shielding</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
         <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="str">
+      <c r="A19" s="2">
         <f>cerebro_data!A19</f>
         <v>1</v>
       </c>
       <c r="B19" t="str">
         <f>cerebro_data!B19</f>
-        <v>Molex MicroClasp socket</v>
+        <v>Micro USB horizontal socket</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1491,33 +1509,33 @@
       </c>
       <c r="B20" t="str">
         <f>cerebro_data!B20</f>
-        <v>Molex MicroClasp plug with wire</v>
+        <v>Molex MicroClasp socket</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
-        <v>0151360206</v>
+        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
       </c>
       <c r="D20" t="str">
         <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="2" t="str">
         <f>cerebro_data!A21</f>
         <v>1</v>
       </c>
       <c r="B21" t="str">
         <f>cerebro_data!B21</f>
-        <v>Red LED (0603)</v>
+        <v>Molex MicroClasp plug with wire</v>
       </c>
       <c r="C21" t="str">
         <f>IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
+        <v>0151360206</v>
       </c>
       <c r="D21" t="str">
         <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1527,230 +1545,248 @@
       </c>
       <c r="B22" t="str">
         <f>cerebro_data!B22</f>
-        <v>Amber LED (0603)</v>
+        <v>Red LED (0603)</v>
       </c>
       <c r="C22" t="str">
         <f>IF(ISBLANK(cerebro_data!D22),cerebro_data!C22,CONCATENATE(" :download:`",cerebro_data!C22,"&lt;Datasheets/",cerebro_data!D22,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
       </c>
       <c r="D22" t="str">
         <f>IF(ISBLANK(cerebro_data!F22),"",CONCATENATE("`",cerebro_data!E22," &lt;",cerebro_data!F22,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="str">
+      <c r="A23" s="2">
         <f>cerebro_data!A23</f>
         <v>1</v>
       </c>
       <c r="B23" t="str">
         <f>cerebro_data!B23</f>
-        <v>470 nF Capacitor (0805)</v>
+        <v>Amber LED (0603)</v>
       </c>
       <c r="C23" t="str">
-        <f>""</f>
-        <v/>
+        <f>IF(ISBLANK(cerebro_data!D23),cerebro_data!C23,CONCATENATE(" :download:`",cerebro_data!C23,"&lt;Datasheets/",cerebro_data!D23,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
       </c>
       <c r="D23" t="str">
         <f>IF(ISBLANK(cerebro_data!F23),"",CONCATENATE("`",cerebro_data!E23," &lt;",cerebro_data!F23,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
         <f>cerebro_data!A24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="str">
         <f>cerebro_data!B24</f>
-        <v>1 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C24" t="str">
-        <f>""</f>
-        <v/>
+        <v>470 nF Capacitor (0805)</v>
+      </c>
+      <c r="C24">
+        <f>IF(ISBLANK(cerebro_data!D24),cerebro_data!C24,CONCATENATE(" :download:`",cerebro_data!C24,"&lt;Datasheets/",cerebro_data!D24,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>IF(ISBLANK(cerebro_data!F24),"",CONCATENATE("`",cerebro_data!E24," &lt;",cerebro_data!F24,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="2" t="str">
         <f>cerebro_data!A25</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="str">
         <f>cerebro_data!B25</f>
-        <v>2.2 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C25" t="str">
-        <f>""</f>
-        <v/>
+        <v>1 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C25">
+        <f>IF(ISBLANK(cerebro_data!D25),cerebro_data!C25,CONCATENATE(" :download:`",cerebro_data!C25,"&lt;Datasheets/",cerebro_data!D25,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>IF(ISBLANK(cerebro_data!F25),"",CONCATENATE("`",cerebro_data!E25," &lt;",cerebro_data!F25,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="str">
+      <c r="A26" s="2">
         <f>cerebro_data!A26</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" t="str">
         <f>cerebro_data!B26</f>
-        <v>10 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C26" t="str">
-        <f>""</f>
-        <v/>
+        <v>2.2 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C26">
+        <f>IF(ISBLANK(cerebro_data!D26),cerebro_data!C26,CONCATENATE(" :download:`",cerebro_data!C26,"&lt;Datasheets/",cerebro_data!D26,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D26" t="str">
         <f>IF(ISBLANK(cerebro_data!F26),"",CONCATENATE("`",cerebro_data!E26," &lt;",cerebro_data!F26,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
         <f>cerebro_data!A27</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="str">
         <f>cerebro_data!B27</f>
-        <v>0.01 |OHgr| Resistor (1206)</v>
-      </c>
-      <c r="C27" t="str">
-        <f>""</f>
-        <v/>
+        <v>10 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C27">
+        <f>IF(ISBLANK(cerebro_data!D27),cerebro_data!C27,CONCATENATE(" :download:`",cerebro_data!C27,"&lt;Datasheets/",cerebro_data!D27,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D27" t="str">
         <f>IF(ISBLANK(cerebro_data!F27),"",CONCATENATE("`",cerebro_data!E27," &lt;",cerebro_data!F27,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
         <f>cerebro_data!A28</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="str">
         <f>cerebro_data!B28</f>
-        <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
-      </c>
-      <c r="C28" t="str">
-        <f>""</f>
-        <v/>
+        <v>0.01 |OHgr| Resistor (1206)</v>
+      </c>
+      <c r="C28">
+        <f>IF(ISBLANK(cerebro_data!D28),cerebro_data!C28,CONCATENATE(" :download:`",cerebro_data!C28,"&lt;Datasheets/",cerebro_data!D28,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D28" t="str">
         <f>IF(ISBLANK(cerebro_data!F28),"",CONCATENATE("`",cerebro_data!E28," &lt;",cerebro_data!F28,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
         <f>cerebro_data!A29</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" t="str">
         <f>cerebro_data!B29</f>
-        <v>27 |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C29" t="str">
-        <f>""</f>
-        <v/>
+        <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
+      </c>
+      <c r="C29">
+        <f>IF(ISBLANK(cerebro_data!D29),cerebro_data!C29,CONCATENATE(" :download:`",cerebro_data!C29,"&lt;Datasheets/",cerebro_data!D29,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D29" t="str">
         <f>IF(ISBLANK(cerebro_data!F29),"",CONCATENATE("`",cerebro_data!E29," &lt;",cerebro_data!F29,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="2" t="str">
         <f>cerebro_data!A30</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B30" t="str">
         <f>cerebro_data!B30</f>
-        <v>2 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C30" t="str">
-        <f>""</f>
-        <v/>
+        <v>27 |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C30">
+        <f>IF(ISBLANK(cerebro_data!D30),cerebro_data!C30,CONCATENATE(" :download:`",cerebro_data!C30,"&lt;Datasheets/",cerebro_data!D30,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D30" t="str">
         <f>IF(ISBLANK(cerebro_data!F30),"",CONCATENATE("`",cerebro_data!E30," &lt;",cerebro_data!F30,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="str">
+      <c r="A31" s="2">
         <f>cerebro_data!A31</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="str">
         <f>cerebro_data!B31</f>
-        <v>4.7 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C31" t="str">
-        <f>""</f>
-        <v/>
+        <v>2 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C31">
+        <f>IF(ISBLANK(cerebro_data!D31),cerebro_data!C31,CONCATENATE(" :download:`",cerebro_data!C31,"&lt;Datasheets/",cerebro_data!D31,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D31" t="str">
         <f>IF(ISBLANK(cerebro_data!F31),"",CONCATENATE("`",cerebro_data!E31," &lt;",cerebro_data!F31,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="2" t="str">
         <f>cerebro_data!A32</f>
         <v>2</v>
       </c>
       <c r="B32" t="str">
         <f>cerebro_data!B32</f>
-        <v>12 k\ |OHgr| Resistor (0805)</v>
-      </c>
-      <c r="C32" t="str">
-        <f>""</f>
-        <v/>
+        <v>4.7 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C32">
+        <f>IF(ISBLANK(cerebro_data!D32),cerebro_data!C32,CONCATENATE(" :download:`",cerebro_data!C32,"&lt;Datasheets/",cerebro_data!D32,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D32" t="str">
         <f>IF(ISBLANK(cerebro_data!F32),"",CONCATENATE("`",cerebro_data!E32," &lt;",cerebro_data!F32,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="str">
+      <c r="A33" s="2">
         <f>cerebro_data!A33</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B33" t="str">
         <f>cerebro_data!B33</f>
-        <v>20 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C33" t="str">
-        <f>""</f>
-        <v/>
+        <v>12 k\ |OHgr| Resistor (0805)</v>
+      </c>
+      <c r="C33">
+        <f>IF(ISBLANK(cerebro_data!D33),cerebro_data!C33,CONCATENATE(" :download:`",cerebro_data!C33,"&lt;Datasheets/",cerebro_data!D33,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D33" t="str">
         <f>IF(ISBLANK(cerebro_data!F33),"",CONCATENATE("`",cerebro_data!E33," &lt;",cerebro_data!F33,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="A34" s="2" t="str">
         <f>cerebro_data!A34</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B34" t="str">
         <f>cerebro_data!B34</f>
-        <v>100 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C34" t="str">
-        <f>""</f>
-        <v/>
+        <v>20 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C34">
+        <f>IF(ISBLANK(cerebro_data!D34),cerebro_data!C34,CONCATENATE(" :download:`",cerebro_data!C34,"&lt;Datasheets/",cerebro_data!D34,"&gt;`"))</f>
+        <v>0</v>
       </c>
       <c r="D34" t="str">
         <f>IF(ISBLANK(cerebro_data!F34),"",CONCATENATE("`",cerebro_data!E34," &lt;",cerebro_data!F34,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <f>cerebro_data!A35</f>
+        <v>2</v>
+      </c>
+      <c r="B35" t="str">
+        <f>cerebro_data!B35</f>
+        <v>100 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C35">
+        <f>IF(ISBLANK(cerebro_data!D35),cerebro_data!C35,CONCATENATE(" :download:`",cerebro_data!C35,"&lt;Datasheets/",cerebro_data!D35,"&gt;`"))</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(ISBLANK(cerebro_data!F35),"",CONCATENATE("`",cerebro_data!E35," &lt;",cerebro_data!F35,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND&gt;`_</v>
       </c>
     </row>
@@ -1767,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC250F28-3064-E743-B78A-8D6381A20273}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1811,17 +1847,17 @@
         <v>89</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1829,37 +1865,37 @@
         <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1867,77 +1903,77 @@
         <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1992,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2041,16 +2077,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>233</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>133</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2138,19 +2174,19 @@
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2294,43 +2330,43 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>56</v>
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2338,19 +2374,19 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2358,39 +2394,39 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="E19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2398,36 +2434,36 @@
         <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2435,41 +2471,47 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>39</v>
@@ -2479,147 +2521,161 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>1</v>
+      <c r="A25" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>182</v>
+      <c r="A26" s="2">
+        <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>202</v>
+        <v>89</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="E33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>2</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>2</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F115" s="3"/>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F116" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3376,16 +3432,16 @@
         <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3544,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC32778-A014-934E-B9C7-1735DC2E5111}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3584,9 +3640,13 @@
         <f>dock_data!B2</f>
         <v>Charging Dock PCB</v>
       </c>
+      <c r="C2" s="7" t="str">
+        <f>IF(ISBLANK(dock_data!C2),"",CONCATENATE(" :download:`",dock_data!C2,"&lt;Datasheets/",dock_data!D2,"&gt;`"))</f>
+        <v xml:space="preserve"> :download:`Charging Dock 2.0&lt;Datasheets/charging_dock_2.0.pdf&gt;`</v>
+      </c>
       <c r="D2" s="7" t="str">
         <f>IF(ISBLANK(dock_data!F2),"",CONCATENATE("`",dock_data!E2," &lt;",dock_data!F2,"&gt;`_"))</f>
-        <v/>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/hz6upCEq&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3766,7 +3826,7 @@
   <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="A1:XFD1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3809,55 +3869,59 @@
         <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>143</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3865,19 +3929,19 @@
         <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3885,67 +3949,67 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3954,10 +4018,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3966,10 +4030,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>

</xml_diff>

<commit_message>
Updates for Cerebro 5.8. Revamped session start dialog. Can now easily connect to any Cerebro and can easily setup new Cerebros.
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3796FAEA-06F3-9A42-B81E-95FAE8E30298}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384C7B66-87FA-F54B-AEBA-B9FDE9DBD842}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="251">
   <si>
     <t>Qty</t>
   </si>
@@ -201,15 +201,6 @@
     <t>ATMEGA32U4-MUR</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=%09401-2012-1-ND</t>
-  </si>
-  <si>
-    <t>slide_switch.pdf</t>
-  </si>
-  <si>
-    <t>AYZ0102AGRLC</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=576-1729-1-ND</t>
   </si>
   <si>
@@ -441,18 +432,12 @@
     <t>Molex MicroClasp socket</t>
   </si>
   <si>
-    <t>Molex MicroClasp plug with wire</t>
-  </si>
-  <si>
     <t>0559350230</t>
   </si>
   <si>
     <t>0151360206</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=wm16380-nd</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=wm12296-nd</t>
   </si>
   <si>
@@ -751,6 +736,60 @@
   </si>
   <si>
     <t>https://oshpark.com/shared_projects/hz6upCEq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Momentary Button</t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t>momentary.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=sw1020ct</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=401-2016-1-nd</t>
+  </si>
+  <si>
+    <t>slide_switch2.pdf</t>
+  </si>
+  <si>
+    <t>PCM12SMTR</t>
+  </si>
+  <si>
+    <t>Green LED (0603)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=511-1578-1-ND</t>
+  </si>
+  <si>
+    <t>led_green.pdf</t>
+  </si>
+  <si>
+    <t>SML-D12M8WT86</t>
+  </si>
+  <si>
+    <t>Molex Micro-Lock plug with wire</t>
+  </si>
+  <si>
+    <t>Molex Micro-Lock socket</t>
+  </si>
+  <si>
+    <t>microlock_plug.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=WM17161-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=WM17038CT-ND</t>
+  </si>
+  <si>
+    <t>microlock_socket.pdf</t>
   </si>
 </sst>
 </file>
@@ -834,7 +873,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -850,6 +889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1148,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,29 +1481,29 @@
       </c>
       <c r="C16" t="str">
         <f>IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`AYZ0102AGRLC&lt;Datasheets/slide_switch.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`PCM12SMTR&lt;Datasheets/slide_switch2.pdf&gt;`</v>
       </c>
       <c r="D16" t="str">
         <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09401-2012-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=401-2016-1-nd&gt;`_</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="2" t="str">
         <f>cerebro_data!A17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="str">
         <f>cerebro_data!B17</f>
-        <v>Micro USB vertical plug</v>
+        <v>Momentary Button</v>
       </c>
       <c r="C17" t="str">
         <f>IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`B3U-1000P&lt;Datasheets/momentary.pdf&gt;`</v>
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=sw1020ct&gt;`_</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1473,15 +1513,15 @@
       </c>
       <c r="B18" t="str">
         <f>cerebro_data!B18</f>
-        <v>Micro USB shielding</v>
+        <v>Micro USB vertical plug</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
         <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1491,33 +1531,33 @@
       </c>
       <c r="B19" t="str">
         <f>cerebro_data!B19</f>
-        <v>Micro USB horizontal socket</v>
+        <v>Micro USB shielding</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
       </c>
       <c r="D19" t="str">
         <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="str">
+      <c r="A20" s="2">
         <f>cerebro_data!A20</f>
         <v>1</v>
       </c>
       <c r="B20" t="str">
         <f>cerebro_data!B20</f>
-        <v>Molex MicroClasp socket</v>
+        <v>Micro USB horizontal socket</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D20" t="str">
         <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1527,33 +1567,33 @@
       </c>
       <c r="B21" t="str">
         <f>cerebro_data!B21</f>
-        <v>Molex MicroClasp plug with wire</v>
+        <v>Molex Micro-Lock socket</v>
       </c>
       <c r="C21" t="str">
         <f>IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
-        <v>0151360206</v>
+        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microlock_socket.pdf&gt;`</v>
       </c>
       <c r="D21" t="str">
         <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm16380-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17038CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="2" t="str">
         <f>cerebro_data!A22</f>
         <v>1</v>
       </c>
       <c r="B22" t="str">
         <f>cerebro_data!B22</f>
-        <v>Red LED (0603)</v>
+        <v>Molex Micro-Lock plug with wire</v>
       </c>
       <c r="C22" t="str">
         <f>IF(ISBLANK(cerebro_data!D22),cerebro_data!C22,CONCATENATE(" :download:`",cerebro_data!C22,"&lt;Datasheets/",cerebro_data!D22,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`0151360206&lt;Datasheets/microlock_plug.pdf&gt;`</v>
       </c>
       <c r="D22" t="str">
         <f>IF(ISBLANK(cerebro_data!F22),"",CONCATENATE("`",cerebro_data!E22," &lt;",cerebro_data!F22,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17161-ND&gt;`_</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1563,213 +1603,212 @@
       </c>
       <c r="B23" t="str">
         <f>cerebro_data!B23</f>
-        <v>Amber LED (0603)</v>
+        <v>Red LED (0603)</v>
       </c>
       <c r="C23" t="str">
         <f>IF(ISBLANK(cerebro_data!D23),cerebro_data!C23,CONCATENATE(" :download:`",cerebro_data!C23,"&lt;Datasheets/",cerebro_data!D23,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
       </c>
       <c r="D23" t="str">
         <f>IF(ISBLANK(cerebro_data!F23),"",CONCATENATE("`",cerebro_data!E23," &lt;",cerebro_data!F23,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="str">
+      <c r="A24" s="2">
         <f>cerebro_data!A24</f>
         <v>1</v>
       </c>
       <c r="B24" t="str">
         <f>cerebro_data!B24</f>
-        <v>470 nF Capacitor (0805)</v>
-      </c>
-      <c r="C24">
+        <v>Amber LED (0603)</v>
+      </c>
+      <c r="C24" t="str">
         <f>IF(ISBLANK(cerebro_data!D24),cerebro_data!C24,CONCATENATE(" :download:`",cerebro_data!C24,"&lt;Datasheets/",cerebro_data!D24,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
       </c>
       <c r="D24" t="str">
         <f>IF(ISBLANK(cerebro_data!F24),"",CONCATENATE("`",cerebro_data!E24," &lt;",cerebro_data!F24,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="str">
+      <c r="A25" s="2">
         <f>cerebro_data!A25</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="str">
         <f>cerebro_data!B25</f>
-        <v>1 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C25">
+        <v>Green LED (0603)</v>
+      </c>
+      <c r="C25" t="str">
         <f>IF(ISBLANK(cerebro_data!D25),cerebro_data!C25,CONCATENATE(" :download:`",cerebro_data!C25,"&lt;Datasheets/",cerebro_data!D25,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> :download:`SML-D12M8WT86&lt;Datasheets/led_green.pdf&gt;`</v>
       </c>
       <c r="D25" t="str">
         <f>IF(ISBLANK(cerebro_data!F25),"",CONCATENATE("`",cerebro_data!E25," &lt;",cerebro_data!F25,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=511-1578-1-ND&gt;`_</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="2" t="str">
         <f>cerebro_data!A26</f>
         <v>1</v>
       </c>
       <c r="B26" t="str">
         <f>cerebro_data!B26</f>
-        <v>2.2 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C26">
+        <v>470 nF Capacitor (0805)</v>
+      </c>
+      <c r="C26" t="str">
         <f>IF(ISBLANK(cerebro_data!D26),cerebro_data!C26,CONCATENATE(" :download:`",cerebro_data!C26,"&lt;Datasheets/",cerebro_data!D26,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D26" t="str">
         <f>IF(ISBLANK(cerebro_data!F26),"",CONCATENATE("`",cerebro_data!E26," &lt;",cerebro_data!F26,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
         <f>cerebro_data!A27</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" t="str">
         <f>cerebro_data!B27</f>
-        <v>10 |mgr|\F Capacitor (0805)</v>
-      </c>
-      <c r="C27">
+        <v>1 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C27" t="str">
         <f>IF(ISBLANK(cerebro_data!D27),cerebro_data!C27,CONCATENATE(" :download:`",cerebro_data!C27,"&lt;Datasheets/",cerebro_data!D27,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D27" t="str">
         <f>IF(ISBLANK(cerebro_data!F27),"",CONCATENATE("`",cerebro_data!E27," &lt;",cerebro_data!F27,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="str">
+      <c r="A28" s="2">
         <f>cerebro_data!A28</f>
         <v>1</v>
       </c>
       <c r="B28" t="str">
         <f>cerebro_data!B28</f>
-        <v>0.01 |OHgr| Resistor (1206)</v>
-      </c>
-      <c r="C28">
+        <v>2.2 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C28" t="str">
         <f>IF(ISBLANK(cerebro_data!D28),cerebro_data!C28,CONCATENATE(" :download:`",cerebro_data!C28,"&lt;Datasheets/",cerebro_data!D28,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D28" t="str">
         <f>IF(ISBLANK(cerebro_data!F28),"",CONCATENATE("`",cerebro_data!E28," &lt;",cerebro_data!F28,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
         <f>cerebro_data!A29</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B29" t="str">
         <f>cerebro_data!B29</f>
-        <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
-      </c>
-      <c r="C29">
+        <v>10 |mgr|\F Capacitor (0805)</v>
+      </c>
+      <c r="C29" t="str">
         <f>IF(ISBLANK(cerebro_data!D29),cerebro_data!C29,CONCATENATE(" :download:`",cerebro_data!C29,"&lt;Datasheets/",cerebro_data!D29,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D29" t="str">
         <f>IF(ISBLANK(cerebro_data!F29),"",CONCATENATE("`",cerebro_data!E29," &lt;",cerebro_data!F29,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
         <f>cerebro_data!A30</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B30" t="str">
         <f>cerebro_data!B30</f>
-        <v>27 |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C30">
+        <v>0.01 |OHgr| Resistor (1206)</v>
+      </c>
+      <c r="C30" t="str">
         <f>IF(ISBLANK(cerebro_data!D30),cerebro_data!C30,CONCATENATE(" :download:`",cerebro_data!C30,"&lt;Datasheets/",cerebro_data!D30,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D30" t="str">
         <f>IF(ISBLANK(cerebro_data!F30),"",CONCATENATE("`",cerebro_data!E30," &lt;",cerebro_data!F30,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="2" t="str">
         <f>cerebro_data!A31</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" t="str">
         <f>cerebro_data!B31</f>
-        <v>2 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C31">
+        <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
+      </c>
+      <c r="C31" t="str">
         <f>IF(ISBLANK(cerebro_data!D31),cerebro_data!C31,CONCATENATE(" :download:`",cerebro_data!C31,"&lt;Datasheets/",cerebro_data!D31,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D31" t="str">
         <f>IF(ISBLANK(cerebro_data!F31),"",CONCATENATE("`",cerebro_data!E31," &lt;",cerebro_data!F31,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
         <f>cerebro_data!A32</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B32" t="str">
         <f>cerebro_data!B32</f>
-        <v>4.7 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C32">
+        <v>27 |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C32" t="str">
         <f>IF(ISBLANK(cerebro_data!D32),cerebro_data!C32,CONCATENATE(" :download:`",cerebro_data!C32,"&lt;Datasheets/",cerebro_data!D32,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D32" t="str">
         <f>IF(ISBLANK(cerebro_data!F32),"",CONCATENATE("`",cerebro_data!E32," &lt;",cerebro_data!F32,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <f>cerebro_data!A33</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" t="str">
         <f>cerebro_data!B33</f>
-        <v>12 k\ |OHgr| Resistor (0805)</v>
-      </c>
-      <c r="C33">
+        <v>2 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C33" t="str">
         <f>IF(ISBLANK(cerebro_data!D33),cerebro_data!C33,CONCATENATE(" :download:`",cerebro_data!C33,"&lt;Datasheets/",cerebro_data!D33,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D33" t="str">
         <f>IF(ISBLANK(cerebro_data!F33),"",CONCATENATE("`",cerebro_data!E33," &lt;",cerebro_data!F33,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="str">
-        <f>cerebro_data!A34</f>
-        <v>6</v>
+      <c r="A34" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="B34" t="str">
         <f>cerebro_data!B34</f>
-        <v>20 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C34">
+        <v>4.7 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C34" t="str">
         <f>IF(ISBLANK(cerebro_data!D34),cerebro_data!C34,CONCATENATE(" :download:`",cerebro_data!C34,"&lt;Datasheets/",cerebro_data!D34,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D34" t="str">
         <f>IF(ISBLANK(cerebro_data!F34),"",CONCATENATE("`",cerebro_data!E34," &lt;",cerebro_data!F34,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1779,14 +1818,49 @@
       </c>
       <c r="B35" t="str">
         <f>cerebro_data!B35</f>
-        <v>100 k\ |OHgr| Resistor (0603)</v>
-      </c>
-      <c r="C35">
+        <v>12 k\ |OHgr| Resistor (0805)</v>
+      </c>
+      <c r="C35" t="str">
         <f>IF(ISBLANK(cerebro_data!D35),cerebro_data!C35,CONCATENATE(" :download:`",cerebro_data!C35,"&lt;Datasheets/",cerebro_data!D35,"&gt;`"))</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D35" t="str">
         <f>IF(ISBLANK(cerebro_data!F35),"",CONCATENATE("`",cerebro_data!E35," &lt;",cerebro_data!F35,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" t="str">
+        <f>cerebro_data!B36</f>
+        <v>20 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C36" t="str">
+        <f>IF(ISBLANK(cerebro_data!D36),cerebro_data!C36,CONCATENATE(" :download:`",cerebro_data!C36,"&lt;Datasheets/",cerebro_data!D36,"&gt;`"))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(ISBLANK(cerebro_data!F36),"",CONCATENATE("`",cerebro_data!E36," &lt;",cerebro_data!F36,"&gt;`_"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <f>cerebro_data!A37</f>
+        <v>2</v>
+      </c>
+      <c r="B37" t="str">
+        <f>cerebro_data!B37</f>
+        <v>100 k\ |OHgr| Resistor (0603)</v>
+      </c>
+      <c r="C37" t="str">
+        <f>IF(ISBLANK(cerebro_data!D37),cerebro_data!C37,CONCATENATE(" :download:`",cerebro_data!C37,"&lt;Datasheets/",cerebro_data!D37,"&gt;`"))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(ISBLANK(cerebro_data!F37),"",CONCATENATE("`",cerebro_data!E37," &lt;",cerebro_data!F37,"&gt;`_"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND&gt;`_</v>
       </c>
     </row>
@@ -1844,136 +1918,136 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2028,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2077,16 +2151,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2100,7 +2174,7 @@
         <v>1570</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>29</v>
@@ -2151,47 +2225,47 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -2277,7 +2351,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
@@ -2286,7 +2360,7 @@
         <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2297,16 +2371,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2317,36 +2391,36 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2357,36 +2431,36 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>240</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>239</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>60</v>
+      <c r="A17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>236</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>59</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2394,19 +2468,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2414,76 +2488,79 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>77</v>
+      <c r="A20" s="2">
+        <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>137</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>1</v>
+      <c r="A22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>44</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2491,173 +2568,212 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>89</v>
+      <c r="A25" s="2">
+        <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>188</v>
+        <v>241</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>1</v>
+      <c r="A26" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>77</v>
+      <c r="A28" s="2">
+        <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>199</v>
+        <v>74</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>1</v>
+      <c r="A31" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2665,17 +2781,54 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F116" s="3"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F118" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2688,7 +2841,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2915,7 +3068,7 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2955,131 +3108,131 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
@@ -3088,35 +3241,35 @@
         <v>39</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>" "</f>
@@ -3128,10 +3281,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>" "</f>
@@ -3426,82 +3579,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3509,27 +3662,27 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3600,7 +3753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC32778-A014-934E-B9C7-1735DC2E5111}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
@@ -3866,82 +4019,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3949,67 +4102,67 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4018,10 +4171,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4030,10 +4183,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>

</xml_diff>

<commit_message>
doc update. Xavier 3.9.0 , base station 2.5, cerebro 5.8
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384C7B66-87FA-F54B-AEBA-B9FDE9DBD842}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBF018B-4277-664B-AE56-3D6CB2792D49}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="23460" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="progammer" sheetId="11" r:id="rId9"/>
     <sheet name="programmer_data" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="252">
   <si>
     <t>Qty</t>
   </si>
@@ -123,12 +123,6 @@
     <t>usb_socket_vertical.pdf</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/13851</t>
-  </si>
-  <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
     <t>https://lowpowerlab.com/shop/product/158</t>
   </si>
   <si>
@@ -441,15 +435,6 @@
     <t>https://www.digikey.com/products/en?keywords=wm12296-nd</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/Ed6Ntbb1</t>
-  </si>
-  <si>
-    <t>Base Station 2.2</t>
-  </si>
-  <si>
-    <t>base_station_2.2.pdf</t>
-  </si>
-  <si>
     <t>Charging Dock PCB</t>
   </si>
   <si>
@@ -723,15 +708,6 @@
     <t>M22-2510805</t>
   </si>
   <si>
-    <t>Cerebro 5.7</t>
-  </si>
-  <si>
-    <t>https://oshpark.com/shared_projects/MiiC2fHG</t>
-  </si>
-  <si>
-    <t>cerebro5.7.pdf</t>
-  </si>
-  <si>
     <t>charging_dock_2.0.pdf</t>
   </si>
   <si>
@@ -790,6 +766,33 @@
   </si>
   <si>
     <t>microlock_socket.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 51 k\ |OHgr| Resistor </t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3898</t>
+  </si>
+  <si>
+    <t>3898</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/ASxhDBJv</t>
+  </si>
+  <si>
+    <t>Cerebro 5.8</t>
+  </si>
+  <si>
+    <t>cerebro5.8.pdf</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/qpPpopqr</t>
+  </si>
+  <si>
+    <t>base_station_2.5.pdf</t>
+  </si>
+  <si>
+    <t>Base Station 2.5</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -1229,11 +1232,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Cerebro 5.7&lt;Datasheets/cerebro5.7.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`Cerebro 5.8&lt;Datasheets/cerebro5.8.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/MiiC2fHG&gt;`_</v>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/ASxhDBJv&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1247,11 +1250,11 @@
       </c>
       <c r="C3" t="str">
         <f>IF(ISBLANK(cerebro_data!D3),cerebro_data!C3,CONCATENATE(" :download:`",cerebro_data!C3,"&lt;Datasheets/",cerebro_data!D3,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`1570&lt;Datasheets/battery_400mah.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`3898&lt;Datasheets/battery_400mah.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
         <f>IF(ISBLANK(cerebro_data!F3),"",CONCATENATE("`",cerebro_data!E3," &lt;",cerebro_data!F3,"&gt;`_"))</f>
-        <v>`Sparkfun &lt;https://www.sparkfun.com/products/13851&gt;`_</v>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/3898&gt;`_</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1796,7 +1799,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B34" t="str">
         <f>cerebro_data!B34</f>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B36" t="str">
         <f>cerebro_data!B36</f>
@@ -1918,136 +1921,136 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2105,7 +2108,7 @@
   <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2134,7 +2137,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>19</v>
@@ -2151,16 +2154,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2170,17 +2173,17 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2">
-        <v>1570</v>
+      <c r="C3" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>214</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2191,16 +2194,16 @@
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2211,76 +2214,76 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2297,10 +2300,10 @@
         <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2311,16 +2314,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2331,16 +2334,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2351,16 +2354,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2371,16 +2374,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2391,36 +2394,36 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2431,36 +2434,36 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2468,19 +2471,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,19 +2491,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2508,59 +2511,59 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2568,19 +2571,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2588,19 +2591,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2608,53 +2611,53 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2662,84 +2665,84 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2747,33 +2750,33 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2781,33 +2784,33 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2815,16 +2818,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="118" spans="6:6" x14ac:dyDescent="0.2">
@@ -3108,168 +3111,168 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>" "</f>
@@ -3281,10 +3284,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>" "</f>
@@ -3373,11 +3376,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(base_data!C2),"",CONCATENATE(" :download:`",base_data!C2,"&lt;Datasheets/",base_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Base Station 2.2&lt;Datasheets/base_station_2.2.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`Base Station 2.5&lt;Datasheets/base_station_2.5.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(base_data!F2),"",CONCATENATE("`",base_data!E2," &lt;",base_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/Ed6Ntbb1&gt;`_</v>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/qpPpopqr&gt;`_</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3459,7 +3462,7 @@
       </c>
       <c r="B7" s="2" t="str">
         <f>base_data!B7</f>
-        <v xml:space="preserve">0603 10 k\ |OHgr| Resistor </v>
+        <v xml:space="preserve">0805 51 k\ |OHgr| Resistor </v>
       </c>
       <c r="C7" t="str">
         <f>IF(ISBLANK(base_data!C7),"",CONCATENATE(" :download:`",base_data!C7,"&lt;Datasheets/",base_data!D7,"&gt;`"))</f>
@@ -3538,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3579,82 +3582,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>134</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3662,27 +3665,27 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -4019,82 +4022,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4102,67 +4105,67 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4171,10 +4174,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4183,10 +4186,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>

</xml_diff>

<commit_message>
added double underscore to links to remove sphinx build warnings about duplicate links added line after github url to remove another build warning edited bom table to account for when a datasheet pdf wasn't provided. this fixes another build error where it was trying to create a download to link to the Download/ directory since no download pdf was appended to the path
</commit_message>
<xml_diff>
--- a/Documentation_src/source/Hardware/tables.xlsx
+++ b/Documentation_src/source/Hardware/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Cerebro/Documentation_src/source/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBF018B-4277-664B-AE56-3D6CB2792D49}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EB0F27-A797-6348-BCFF-8441CD36FEF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="23460" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cerebro" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="249">
   <si>
     <t>Qty</t>
   </si>
@@ -420,21 +425,9 @@
     <t xml:space="preserve">0603 10 k\ |OHgr| Resistor </t>
   </si>
   <si>
-    <t>microclasp.pdf</t>
-  </si>
-  <si>
-    <t>Molex MicroClasp socket</t>
-  </si>
-  <si>
-    <t>0559350230</t>
-  </si>
-  <si>
     <t>0151360206</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=wm12296-nd</t>
-  </si>
-  <si>
     <t>Charging Dock PCB</t>
   </si>
   <si>
@@ -793,6 +786,9 @@
   </si>
   <si>
     <t>Base Station 2.5</t>
+  </si>
+  <si>
+    <t>5055670271</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1231,12 +1227,12 @@
         <v>Cerebro PCB</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C2),"",IF(ISBLANK(cerebro_data!D2),cerebro_data!C2,CONCATENATE(" :download:`",cerebro_data!C2,"&lt;Datasheets/",cerebro_data!D2,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`Cerebro 5.8&lt;Datasheets/cerebro5.8.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/ASxhDBJv&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F2),"",CONCATENATE("`",cerebro_data!E2," &lt;",cerebro_data!F2,"&gt;`__"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/ASxhDBJv&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1249,12 +1245,12 @@
         <v>400 mAh Battery</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(cerebro_data!D3),cerebro_data!C3,CONCATENATE(" :download:`",cerebro_data!C3,"&lt;Datasheets/",cerebro_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C3),"",IF(ISBLANK(cerebro_data!D3),cerebro_data!C3,CONCATENATE(" :download:`",cerebro_data!C3,"&lt;Datasheets/",cerebro_data!D3,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`3898&lt;Datasheets/battery_400mah.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(ISBLANK(cerebro_data!F3),"",CONCATENATE("`",cerebro_data!E3," &lt;",cerebro_data!F3,"&gt;`_"))</f>
-        <v>`Adafruit &lt;https://www.adafruit.com/product/3898&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F3),"",CONCATENATE("`",cerebro_data!E3," &lt;",cerebro_data!F3,"&gt;`__"))</f>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/3898&gt;`__</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1267,12 +1263,12 @@
         <v>915 MHz Radio</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(cerebro_data!D4),cerebro_data!C4,CONCATENATE(" :download:`",cerebro_data!C4,"&lt;Datasheets/",cerebro_data!D4,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C4),"",IF(ISBLANK(cerebro_data!D4),cerebro_data!C4,CONCATENATE(" :download:`",cerebro_data!C4,"&lt;Datasheets/",cerebro_data!D4,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`RFM69HCW&lt;Datasheets/radio.pdf&gt;`</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(ISBLANK(cerebro_data!F4),"",CONCATENATE("`",cerebro_data!E4," &lt;",cerebro_data!F4,"&gt;`_"))</f>
-        <v>`LowPowerLab &lt;https://lowpowerlab.com/shop/product/158&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F4),"",CONCATENATE("`",cerebro_data!E4," &lt;",cerebro_data!F4,"&gt;`__"))</f>
+        <v>`LowPowerLab &lt;https://lowpowerlab.com/shop/product/158&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1285,12 +1281,12 @@
         <v>Microcontroller</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(cerebro_data!D5),cerebro_data!C5,CONCATENATE(" :download:`",cerebro_data!C5,"&lt;Datasheets/",cerebro_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C5),"",IF(ISBLANK(cerebro_data!D5),cerebro_data!C5,CONCATENATE(" :download:`",cerebro_data!C5,"&lt;Datasheets/",cerebro_data!D5,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`ATMEGA32U4-MUR&lt;Datasheets/MCU_32u4.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK(cerebro_data!F5),"",CONCATENATE("`",cerebro_data!E5," &lt;",cerebro_data!F5,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=ATMEGA32U4-MURCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F5),"",CONCATENATE("`",cerebro_data!E5," &lt;",cerebro_data!F5,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=ATMEGA32U4-MURCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1303,12 +1299,12 @@
         <v>8 MHz Resonator</v>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(cerebro_data!D6),cerebro_data!C6,CONCATENATE(" :download:`",cerebro_data!C6,"&lt;Datasheets/",cerebro_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C6),"",IF(ISBLANK(cerebro_data!D6),cerebro_data!C6,CONCATENATE(" :download:`",cerebro_data!C6,"&lt;Datasheets/",cerebro_data!D6,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`CSTCE8M00G55-R0&lt;Datasheets/resonator_8mhz.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(ISBLANK(cerebro_data!F6),"",CONCATENATE("`",cerebro_data!E6," &lt;",cerebro_data!F6,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-1195-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F6),"",CONCATENATE("`",cerebro_data!E6," &lt;",cerebro_data!F6,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-1195-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1321,12 +1317,12 @@
         <v>3.3V Linear Regulator</v>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(cerebro_data!D7),cerebro_data!C7,CONCATENATE(" :download:`",cerebro_data!C7,"&lt;Datasheets/",cerebro_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C7),"",IF(ISBLANK(cerebro_data!D7),cerebro_data!C7,CONCATENATE(" :download:`",cerebro_data!C7,"&lt;Datasheets/",cerebro_data!D7,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`AP2112K-3.3TRG1&lt;Datasheets/regulator_3v_linear.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(ISBLANK(cerebro_data!F7),"",CONCATENATE("`",cerebro_data!E7," &lt;",cerebro_data!F7,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09AP2112K-3.3TRG1DICT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F7),"",CONCATENATE("`",cerebro_data!E7," &lt;",cerebro_data!F7,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09AP2112K-3.3TRG1DICT-ND&gt;`__</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1339,12 +1335,12 @@
         <v>Fuel Gauge</v>
       </c>
       <c r="C8" t="str">
-        <f>IF(ISBLANK(cerebro_data!D8),cerebro_data!C8,CONCATENATE(" :download:`",cerebro_data!C8,"&lt;Datasheets/",cerebro_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C8),"",IF(ISBLANK(cerebro_data!D8),cerebro_data!C8,CONCATENATE(" :download:`",cerebro_data!C8,"&lt;Datasheets/",cerebro_data!D8,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`BQ27441DRZR-G1B&lt;Datasheets/fuel_gauge.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
-        <f>IF(ISBLANK(cerebro_data!F8),"",CONCATENATE("`",cerebro_data!E8," &lt;",cerebro_data!F8,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/texas-instruments/BQ27441DRZR-G1B/296-39942-1-ND/5177819&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F8),"",CONCATENATE("`",cerebro_data!E8," &lt;",cerebro_data!F8,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/texas-instruments/BQ27441DRZR-G1B/296-39942-1-ND/5177819&gt;`__</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1357,12 +1353,12 @@
         <v>DAC (12-Bit)</v>
       </c>
       <c r="C9" t="str">
-        <f>IF(ISBLANK(cerebro_data!D9),cerebro_data!C9,CONCATENATE(" :download:`",cerebro_data!C9,"&lt;Datasheets/",cerebro_data!D9,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C9),"",IF(ISBLANK(cerebro_data!D9),cerebro_data!C9,CONCATENATE(" :download:`",cerebro_data!C9,"&lt;Datasheets/",cerebro_data!D9,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`LTC2630ACSC6-LZ12#TRMPBF&lt;Datasheets/DAC.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
-        <f>IF(ISBLANK(cerebro_data!F9),"",CONCATENATE("`",cerebro_data!E9," &lt;",cerebro_data!F9,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/linear-technology/LTC2630ACSC6-LZ12-TRMPBF/LTC2630ACSC6-LZ12-TRMPBFCT-ND/1643783&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F9),"",CONCATENATE("`",cerebro_data!E9," &lt;",cerebro_data!F9,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/linear-technology/LTC2630ACSC6-LZ12-TRMPBF/LTC2630ACSC6-LZ12-TRMPBFCT-ND/1643783&gt;`__</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1375,12 +1371,12 @@
         <v>Op Amp</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(cerebro_data!D10),cerebro_data!C10,CONCATENATE(" :download:`",cerebro_data!C10,"&lt;Datasheets/",cerebro_data!D10,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C10),"",IF(ISBLANK(cerebro_data!D10),cerebro_data!C10,CONCATENATE(" :download:`",cerebro_data!C10,"&lt;Datasheets/",cerebro_data!D10,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`OPA237NA/3K&lt;Datasheets/opamp.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
-        <f>IF(ISBLANK(cerebro_data!F10),"",CONCATENATE("`",cerebro_data!E10," &lt;",cerebro_data!F10,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-26265-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F10),"",CONCATENATE("`",cerebro_data!E10," &lt;",cerebro_data!F10,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-26265-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1393,12 +1389,12 @@
         <v>NPN Transistor</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(ISBLANK(cerebro_data!D11),cerebro_data!C11,CONCATENATE(" :download:`",cerebro_data!C11,"&lt;Datasheets/",cerebro_data!D11,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C11),"",IF(ISBLANK(cerebro_data!D11),cerebro_data!C11,CONCATENATE(" :download:`",cerebro_data!C11,"&lt;Datasheets/",cerebro_data!D11,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`FJX3904TF&lt;Datasheets/npn_transistor.pdf&gt;`</v>
       </c>
       <c r="D11" t="str">
-        <f>IF(ISBLANK(cerebro_data!F11),"",CONCATENATE("`",cerebro_data!E11," &lt;",cerebro_data!F11,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=FJX3904TFCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F11),"",CONCATENATE("`",cerebro_data!E11," &lt;",cerebro_data!F11,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=FJX3904TFCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1411,12 +1407,12 @@
         <v>Boost Converter</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(ISBLANK(cerebro_data!D12),cerebro_data!C12,CONCATENATE(" :download:`",cerebro_data!C12,"&lt;Datasheets/",cerebro_data!D12,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C12),"",IF(ISBLANK(cerebro_data!D12),cerebro_data!C12,CONCATENATE(" :download:`",cerebro_data!C12,"&lt;Datasheets/",cerebro_data!D12,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`MIC2288YD5-TR&lt;Datasheets/boost_converter.pdf&gt;`</v>
       </c>
       <c r="D12" t="str">
-        <f>IF(ISBLANK(cerebro_data!F12),"",CONCATENATE("`",cerebro_data!E12," &lt;",cerebro_data!F12,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=576-1729-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F12),"",CONCATENATE("`",cerebro_data!E12," &lt;",cerebro_data!F12,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=576-1729-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,12 +1425,12 @@
         <v>Schottky Diode</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(ISBLANK(cerebro_data!D13),cerebro_data!C13,CONCATENATE(" :download:`",cerebro_data!C13,"&lt;Datasheets/",cerebro_data!D13,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C13),"",IF(ISBLANK(cerebro_data!D13),cerebro_data!C13,CONCATENATE(" :download:`",cerebro_data!C13,"&lt;Datasheets/",cerebro_data!D13,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`MBRM140T3G&lt;Datasheets/schottky.pdf&gt;`</v>
       </c>
       <c r="D13" t="str">
-        <f>IF(ISBLANK(cerebro_data!F13),"",CONCATENATE("`",cerebro_data!E13," &lt;",cerebro_data!F13,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=MBRM140T3GOSCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F13),"",CONCATENATE("`",cerebro_data!E13," &lt;",cerebro_data!F13,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=MBRM140T3GOSCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1447,12 +1443,12 @@
         <v>10uH Inductor</v>
       </c>
       <c r="C14" t="str">
-        <f>IF(ISBLANK(cerebro_data!D14),cerebro_data!C14,CONCATENATE(" :download:`",cerebro_data!C14,"&lt;Datasheets/",cerebro_data!D14,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C14),"",IF(ISBLANK(cerebro_data!D14),cerebro_data!C14,CONCATENATE(" :download:`",cerebro_data!C14,"&lt;Datasheets/",cerebro_data!D14,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`LQH43CN100K03L&lt;Datasheets/inductor.pdf&gt;`</v>
       </c>
       <c r="D14" t="str">
-        <f>IF(ISBLANK(cerebro_data!F14),"",CONCATENATE("`",cerebro_data!E14," &lt;",cerebro_data!F14,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-2519-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F14),"",CONCATENATE("`",cerebro_data!E14," &lt;",cerebro_data!F14,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=490-2519-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1465,12 +1461,12 @@
         <v>2mm Pitch Male Header</v>
       </c>
       <c r="C15" t="str">
-        <f>IF(ISBLANK(cerebro_data!D15),cerebro_data!C15,CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C15),"",IF(ISBLANK(cerebro_data!D15),cerebro_data!C15,CONCATENATE(" :download:`",cerebro_data!C15,"&lt;Datasheets/",cerebro_data!D15,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`M22-2510805&lt;Datasheets/header_male_2mm.pdf&gt;`</v>
       </c>
       <c r="D15" t="str">
-        <f>IF(ISBLANK(cerebro_data!F15),"",CONCATENATE("`",cerebro_data!E15," &lt;",cerebro_data!F15,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=952-1992-nd&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F15),"",CONCATENATE("`",cerebro_data!E15," &lt;",cerebro_data!F15,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=952-1992-nd&gt;`__</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,12 +1479,12 @@
         <v>Slide Switch</v>
       </c>
       <c r="C16" t="str">
-        <f>IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C16),"",IF(ISBLANK(cerebro_data!D16),cerebro_data!C16,CONCATENATE(" :download:`",cerebro_data!C16,"&lt;Datasheets/",cerebro_data!D16,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`PCM12SMTR&lt;Datasheets/slide_switch2.pdf&gt;`</v>
       </c>
       <c r="D16" t="str">
-        <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=401-2016-1-nd&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F16),"",CONCATENATE("`",cerebro_data!E16," &lt;",cerebro_data!F16,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=401-2016-1-nd&gt;`__</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1501,12 +1497,12 @@
         <v>Momentary Button</v>
       </c>
       <c r="C17" t="str">
-        <f>IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C17),"",IF(ISBLANK(cerebro_data!D17),cerebro_data!C17,CONCATENATE(" :download:`",cerebro_data!C17,"&lt;Datasheets/",cerebro_data!D17,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`B3U-1000P&lt;Datasheets/momentary.pdf&gt;`</v>
       </c>
       <c r="D17" t="str">
-        <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=sw1020ct&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F17),"",CONCATENATE("`",cerebro_data!E17," &lt;",cerebro_data!F17,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=sw1020ct&gt;`__</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1519,12 +1515,12 @@
         <v>Micro USB vertical plug</v>
       </c>
       <c r="C18" t="str">
-        <f>IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C18),"",IF(ISBLANK(cerebro_data!D18),cerebro_data!C18,CONCATENATE(" :download:`",cerebro_data!C18,"&lt;Datasheets/",cerebro_data!D18,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`ZX20-B-5S-UNIT(30)&lt;Datasheets/usb_plug_vertical.pdf&gt;`</v>
       </c>
       <c r="D18" t="str">
-        <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F18),"",CONCATENATE("`",cerebro_data!E18," &lt;",cerebro_data!F18,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H125237-ND&gt;`__</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1537,12 +1533,12 @@
         <v>Micro USB shielding</v>
       </c>
       <c r="C19" t="str">
-        <f>IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C19),"",IF(ISBLANK(cerebro_data!D19),cerebro_data!C19,CONCATENATE(" :download:`",cerebro_data!C19,"&lt;Datasheets/",cerebro_data!D19,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`ZX20-B-SLDC&lt;Datasheets/usb_shielding.pdf&gt;`</v>
       </c>
       <c r="D19" t="str">
-        <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F19),"",CONCATENATE("`",cerebro_data!E19," &lt;",cerebro_data!F19,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=H11496CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1555,12 +1551,12 @@
         <v>Micro USB horizontal socket</v>
       </c>
       <c r="C20" t="str">
-        <f>IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C20),"",IF(ISBLANK(cerebro_data!D20),cerebro_data!C20,CONCATENATE(" :download:`",cerebro_data!C20,"&lt;Datasheets/",cerebro_data!D20,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D20" t="str">
-        <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F20),"",CONCATENATE("`",cerebro_data!E20," &lt;",cerebro_data!F20,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1573,12 +1569,12 @@
         <v>Molex Micro-Lock socket</v>
       </c>
       <c r="C21" t="str">
-        <f>IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microlock_socket.pdf&gt;`</v>
+        <f>IF(ISBLANK(cerebro_data!C21),"",IF(ISBLANK(cerebro_data!D21),cerebro_data!C21,CONCATENATE(" :download:`",cerebro_data!C21,"&lt;Datasheets/",cerebro_data!D21,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`5055670271&lt;Datasheets/microlock_socket.pdf&gt;`</v>
       </c>
       <c r="D21" t="str">
-        <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17038CT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F21),"",CONCATENATE("`",cerebro_data!E21," &lt;",cerebro_data!F21,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17038CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1591,12 +1587,12 @@
         <v>Molex Micro-Lock plug with wire</v>
       </c>
       <c r="C22" t="str">
-        <f>IF(ISBLANK(cerebro_data!D22),cerebro_data!C22,CONCATENATE(" :download:`",cerebro_data!C22,"&lt;Datasheets/",cerebro_data!D22,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C22),"",IF(ISBLANK(cerebro_data!D22),cerebro_data!C22,CONCATENATE(" :download:`",cerebro_data!C22,"&lt;Datasheets/",cerebro_data!D22,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`0151360206&lt;Datasheets/microlock_plug.pdf&gt;`</v>
       </c>
       <c r="D22" t="str">
-        <f>IF(ISBLANK(cerebro_data!F22),"",CONCATENATE("`",cerebro_data!E22," &lt;",cerebro_data!F22,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17161-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F22),"",CONCATENATE("`",cerebro_data!E22," &lt;",cerebro_data!F22,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17161-ND&gt;`__</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1609,12 +1605,12 @@
         <v>Red LED (0603)</v>
       </c>
       <c r="C23" t="str">
-        <f>IF(ISBLANK(cerebro_data!D23),cerebro_data!C23,CONCATENATE(" :download:`",cerebro_data!C23,"&lt;Datasheets/",cerebro_data!D23,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C23),"",IF(ISBLANK(cerebro_data!D23),cerebro_data!C23,CONCATENATE(" :download:`",cerebro_data!C23,"&lt;Datasheets/",cerebro_data!D23,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`LTST-C191KRKT&lt;Datasheets/led_red.pdf&gt;`</v>
       </c>
       <c r="D23" t="str">
-        <f>IF(ISBLANK(cerebro_data!F23),"",CONCATENATE("`",cerebro_data!E23," &lt;",cerebro_data!F23,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F23),"",CONCATENATE("`",cerebro_data!E23," &lt;",cerebro_data!F23,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=160-1447-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1627,12 +1623,12 @@
         <v>Amber LED (0603)</v>
       </c>
       <c r="C24" t="str">
-        <f>IF(ISBLANK(cerebro_data!D24),cerebro_data!C24,CONCATENATE(" :download:`",cerebro_data!C24,"&lt;Datasheets/",cerebro_data!D24,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C24),"",IF(ISBLANK(cerebro_data!D24),cerebro_data!C24,CONCATENATE(" :download:`",cerebro_data!C24,"&lt;Datasheets/",cerebro_data!D24,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`LNJ437W84RA&lt;Datasheets/led_amber.pdf&gt;`</v>
       </c>
       <c r="D24" t="str">
-        <f>IF(ISBLANK(cerebro_data!F24),"",CONCATENATE("`",cerebro_data!E24," &lt;",cerebro_data!F24,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F24),"",CONCATENATE("`",cerebro_data!E24," &lt;",cerebro_data!F24,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09LNJ437W84RACT-ND&gt;`__</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1645,12 +1641,12 @@
         <v>Green LED (0603)</v>
       </c>
       <c r="C25" t="str">
-        <f>IF(ISBLANK(cerebro_data!D25),cerebro_data!C25,CONCATENATE(" :download:`",cerebro_data!C25,"&lt;Datasheets/",cerebro_data!D25,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C25),"",IF(ISBLANK(cerebro_data!D25),cerebro_data!C25,CONCATENATE(" :download:`",cerebro_data!C25,"&lt;Datasheets/",cerebro_data!D25,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`SML-D12M8WT86&lt;Datasheets/led_green.pdf&gt;`</v>
       </c>
       <c r="D25" t="str">
-        <f>IF(ISBLANK(cerebro_data!F25),"",CONCATENATE("`",cerebro_data!E25," &lt;",cerebro_data!F25,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=511-1578-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F25),"",CONCATENATE("`",cerebro_data!E25," &lt;",cerebro_data!F25,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=511-1578-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1663,12 +1659,12 @@
         <v>470 nF Capacitor (0805)</v>
       </c>
       <c r="C26" t="str">
-        <f>IF(ISBLANK(cerebro_data!D26),cerebro_data!C26,CONCATENATE(" :download:`",cerebro_data!C26,"&lt;Datasheets/",cerebro_data!D26,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C26),"",IF(ISBLANK(cerebro_data!D26),cerebro_data!C26,CONCATENATE(" :download:`",cerebro_data!C26,"&lt;Datasheets/",cerebro_data!D26,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D26" t="str">
-        <f>IF(ISBLANK(cerebro_data!F26),"",CONCATENATE("`",cerebro_data!E26," &lt;",cerebro_data!F26,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F26),"",CONCATENATE("`",cerebro_data!E26," &lt;",cerebro_data!F26,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/avx-corporation/08055C474KAT2A/478-5033-1-ND/1888244&gt;`__</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1681,12 +1677,12 @@
         <v>1 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C27" t="str">
-        <f>IF(ISBLANK(cerebro_data!D27),cerebro_data!C27,CONCATENATE(" :download:`",cerebro_data!C27,"&lt;Datasheets/",cerebro_data!D27,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C27),"",IF(ISBLANK(cerebro_data!D27),cerebro_data!C27,CONCATENATE(" :download:`",cerebro_data!C27,"&lt;Datasheets/",cerebro_data!D27,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D27" t="str">
-        <f>IF(ISBLANK(cerebro_data!F27),"",CONCATENATE("`",cerebro_data!E27," &lt;",cerebro_data!F27,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F27),"",CONCATENATE("`",cerebro_data!E27," &lt;",cerebro_data!F27,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1066-1-nd&gt;`__</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1699,12 +1695,12 @@
         <v>2.2 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C28" t="str">
-        <f>IF(ISBLANK(cerebro_data!D28),cerebro_data!C28,CONCATENATE(" :download:`",cerebro_data!C28,"&lt;Datasheets/",cerebro_data!D28,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C28),"",IF(ISBLANK(cerebro_data!D28),cerebro_data!C28,CONCATENATE(" :download:`",cerebro_data!C28,"&lt;Datasheets/",cerebro_data!D28,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D28" t="str">
-        <f>IF(ISBLANK(cerebro_data!F28),"",CONCATENATE("`",cerebro_data!E28," &lt;",cerebro_data!F28,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F28),"",CONCATENATE("`",cerebro_data!E28," &lt;",cerebro_data!F28,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=587-1286-1&gt;`__</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1717,12 +1713,12 @@
         <v>10 |mgr|\F Capacitor (0805)</v>
       </c>
       <c r="C29" t="str">
-        <f>IF(ISBLANK(cerebro_data!D29),cerebro_data!C29,CONCATENATE(" :download:`",cerebro_data!C29,"&lt;Datasheets/",cerebro_data!D29,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C29),"",IF(ISBLANK(cerebro_data!D29),cerebro_data!C29,CONCATENATE(" :download:`",cerebro_data!C29,"&lt;Datasheets/",cerebro_data!D29,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D29" t="str">
-        <f>IF(ISBLANK(cerebro_data!F29),"",CONCATENATE("`",cerebro_data!E29," &lt;",cerebro_data!F29,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F29),"",CONCATENATE("`",cerebro_data!E29," &lt;",cerebro_data!F29,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BR61E106KA73L/490-5523-1-ND/2334919&gt;`__</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1735,12 +1731,12 @@
         <v>0.01 |OHgr| Resistor (1206)</v>
       </c>
       <c r="C30" t="str">
-        <f>IF(ISBLANK(cerebro_data!D30),cerebro_data!C30,CONCATENATE(" :download:`",cerebro_data!C30,"&lt;Datasheets/",cerebro_data!D30,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C30),"",IF(ISBLANK(cerebro_data!D30),cerebro_data!C30,CONCATENATE(" :download:`",cerebro_data!C30,"&lt;Datasheets/",cerebro_data!D30,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D30" t="str">
-        <f>IF(ISBLANK(cerebro_data!F30),"",CONCATENATE("`",cerebro_data!E30," &lt;",cerebro_data!F30,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F30),"",CONCATENATE("`",cerebro_data!E30," &lt;",cerebro_data!F30,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P0.01BVCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1753,12 +1749,12 @@
         <v xml:space="preserve">12 |OHgr| Resistor (0603) </v>
       </c>
       <c r="C31" t="str">
-        <f>IF(ISBLANK(cerebro_data!D31),cerebro_data!C31,CONCATENATE(" :download:`",cerebro_data!C31,"&lt;Datasheets/",cerebro_data!D31,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C31),"",IF(ISBLANK(cerebro_data!D31),cerebro_data!C31,CONCATENATE(" :download:`",cerebro_data!C31,"&lt;Datasheets/",cerebro_data!D31,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D31" t="str">
-        <f>IF(ISBLANK(cerebro_data!F31),"",CONCATENATE("`",cerebro_data!E31," &lt;",cerebro_data!F31,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F31),"",CONCATENATE("`",cerebro_data!E31," &lt;",cerebro_data!F31,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=P12.00BYCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1771,12 +1767,12 @@
         <v>27 |OHgr| Resistor (0603)</v>
       </c>
       <c r="C32" t="str">
-        <f>IF(ISBLANK(cerebro_data!D32),cerebro_data!C32,CONCATENATE(" :download:`",cerebro_data!C32,"&lt;Datasheets/",cerebro_data!D32,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C32),"",IF(ISBLANK(cerebro_data!D32),cerebro_data!C32,CONCATENATE(" :download:`",cerebro_data!C32,"&lt;Datasheets/",cerebro_data!D32,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D32" t="str">
-        <f>IF(ISBLANK(cerebro_data!F32),"",CONCATENATE("`",cerebro_data!E32," &lt;",cerebro_data!F32,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F32),"",CONCATENATE("`",cerebro_data!E32," &lt;",cerebro_data!F32,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=541-27.0SCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1789,29 +1785,29 @@
         <v>2 k\ |OHgr| Resistor (0603)</v>
       </c>
       <c r="C33" t="str">
-        <f>IF(ISBLANK(cerebro_data!D33),cerebro_data!C33,CONCATENATE(" :download:`",cerebro_data!C33,"&lt;Datasheets/",cerebro_data!D33,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C33),"",IF(ISBLANK(cerebro_data!D33),cerebro_data!C33,CONCATENATE(" :download:`",cerebro_data!C33,"&lt;Datasheets/",cerebro_data!D33,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D33" t="str">
-        <f>IF(ISBLANK(cerebro_data!F33),"",CONCATENATE("`",cerebro_data!E33," &lt;",cerebro_data!F33,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F33),"",CONCATENATE("`",cerebro_data!E33," &lt;",cerebro_data!F33,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD2K00CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B34" t="str">
         <f>cerebro_data!B34</f>
         <v>4.7 k\ |OHgr| Resistor (0603)</v>
       </c>
       <c r="C34" t="str">
-        <f>IF(ISBLANK(cerebro_data!D34),cerebro_data!C34,CONCATENATE(" :download:`",cerebro_data!C34,"&lt;Datasheets/",cerebro_data!D34,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C34),"",IF(ISBLANK(cerebro_data!D34),cerebro_data!C34,CONCATENATE(" :download:`",cerebro_data!C34,"&lt;Datasheets/",cerebro_data!D34,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" t="str">
-        <f>IF(ISBLANK(cerebro_data!F34),"",CONCATENATE("`",cerebro_data!E34," &lt;",cerebro_data!F34,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F34),"",CONCATENATE("`",cerebro_data!E34," &lt;",cerebro_data!F34,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-4.70KHRCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1824,29 +1820,29 @@
         <v>12 k\ |OHgr| Resistor (0805)</v>
       </c>
       <c r="C35" t="str">
-        <f>IF(ISBLANK(cerebro_data!D35),cerebro_data!C35,CONCATENATE(" :download:`",cerebro_data!C35,"&lt;Datasheets/",cerebro_data!D35,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C35),"",IF(ISBLANK(cerebro_data!D35),cerebro_data!C35,CONCATENATE(" :download:`",cerebro_data!C35,"&lt;Datasheets/",cerebro_data!D35,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D35" t="str">
-        <f>IF(ISBLANK(cerebro_data!F35),"",CONCATENATE("`",cerebro_data!E35," &lt;",cerebro_data!F35,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F35),"",CONCATENATE("`",cerebro_data!E35," &lt;",cerebro_data!F35,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=311-12.0KCRCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B36" t="str">
         <f>cerebro_data!B36</f>
         <v>20 k\ |OHgr| Resistor (0603)</v>
       </c>
       <c r="C36" t="str">
-        <f>IF(ISBLANK(cerebro_data!D36),cerebro_data!C36,CONCATENATE(" :download:`",cerebro_data!C36,"&lt;Datasheets/",cerebro_data!D36,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C36),"",IF(ISBLANK(cerebro_data!D36),cerebro_data!C36,CONCATENATE(" :download:`",cerebro_data!C36,"&lt;Datasheets/",cerebro_data!D36,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D36" t="str">
-        <f>IF(ISBLANK(cerebro_data!F36),"",CONCATENATE("`",cerebro_data!E36," &lt;",cerebro_data!F36,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F36),"",CONCATENATE("`",cerebro_data!E36," &lt;",cerebro_data!F36,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=RNCP0603FTD20K0CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1859,12 +1855,12 @@
         <v>100 k\ |OHgr| Resistor (0603)</v>
       </c>
       <c r="C37" t="str">
-        <f>IF(ISBLANK(cerebro_data!D37),cerebro_data!C37,CONCATENATE(" :download:`",cerebro_data!C37,"&lt;Datasheets/",cerebro_data!D37,"&gt;`"))</f>
+        <f>IF(ISBLANK(cerebro_data!C37),"",IF(ISBLANK(cerebro_data!D37),cerebro_data!C37,CONCATENATE(" :download:`",cerebro_data!C37,"&lt;Datasheets/",cerebro_data!D37,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D37" t="str">
-        <f>IF(ISBLANK(cerebro_data!F37),"",CONCATENATE("`",cerebro_data!E37," &lt;",cerebro_data!F37,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(cerebro_data!F37),"",CONCATENATE("`",cerebro_data!E37," &lt;",cerebro_data!F37,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09311-100KHRCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="74" hidden="1" x14ac:dyDescent="0.2"/>
@@ -1924,17 +1920,17 @@
         <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1942,37 +1938,37 @@
         <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1980,77 +1976,77 @@
         <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2108,7 +2104,7 @@
   <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2154,16 +2150,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2174,16 +2170,16 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2251,19 +2247,19 @@
         <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2411,19 +2407,19 @@
         <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2434,16 +2430,16 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2451,19 +2447,19 @@
         <v>84</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2531,19 +2527,19 @@
         <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2551,19 +2547,19 @@
         <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2571,7 +2567,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>69</v>
@@ -2591,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>70</v>
@@ -2611,19 +2607,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2631,16 +2627,16 @@
         <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2648,16 +2644,16 @@
         <v>84</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2665,33 +2661,33 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2699,16 +2695,16 @@
         <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2716,33 +2712,33 @@
         <v>84</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2750,16 +2746,16 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2767,16 +2763,16 @@
         <v>84</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2784,33 +2780,33 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2818,16 +2814,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" spans="6:6" x14ac:dyDescent="0.2">
@@ -2844,7 +2840,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2883,12 +2879,12 @@
         <v>Implant PCB</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(implant_data!D2),implant_data!C2,CONCATENATE(" :download:`",implant_data!C2,"&lt;Datasheets/",implant_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C2),"",IF(ISBLANK(implant_data!D2),implant_data!C2,CONCATENATE(" :download:`",implant_data!C2,"&lt;Datasheets/",implant_data!D2,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`Implant 5.3&lt;Datasheets/implant_5.3.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISBLANK(implant_data!F2),"",CONCATENATE("`",implant_data!E2," &lt;",implant_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/k8Ikpli6&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F2),"",CONCATENATE("`",implant_data!E2," &lt;",implant_data!F2,"&gt;`__"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/k8Ikpli6&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2901,12 +2897,12 @@
         <v>Laser Diode</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(implant_data!D3),implant_data!C3,CONCATENATE(" :download:`",implant_data!C3,"&lt;Datasheets/",implant_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C3),"",IF(ISBLANK(implant_data!D3),implant_data!C3,CONCATENATE(" :download:`",implant_data!C3,"&lt;Datasheets/",implant_data!D3,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`PLT5 520_B1_2_3&lt;Datasheets/green_laser_diode.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(ISBLANK(implant_data!F3),"",CONCATENATE("`",implant_data!E3," &lt;",implant_data!F3,"&gt;`_"))</f>
-        <v>`World Star Tech &lt;http://www.worldstartech.com/products/laser-diodes/green-laser-diode-osram/&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F3),"",CONCATENATE("`",implant_data!E3," &lt;",implant_data!F3,"&gt;`__"))</f>
+        <v>`World Star Tech &lt;http://www.worldstartech.com/products/laser-diodes/green-laser-diode-osram/&gt;`__</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2919,12 +2915,12 @@
         <v>Fiber</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(implant_data!D4),implant_data!C4,CONCATENATE(" :download:`",implant_data!C4,"&lt;Datasheets/",implant_data!D4,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C4),"",IF(ISBLANK(implant_data!D4),implant_data!C4,CONCATENATE(" :download:`",implant_data!C4,"&lt;Datasheets/",implant_data!D4,"&gt;`")))</f>
         <v>F-MBB</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(ISBLANK(implant_data!F4),"",CONCATENATE("`",implant_data!E4," &lt;",implant_data!F4,"&gt;`_"))</f>
-        <v>`Newport &lt;https://www.newport.com/p/F-MBB&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F4),"",CONCATENATE("`",implant_data!E4," &lt;",implant_data!F4,"&gt;`__"))</f>
+        <v>`Newport &lt;https://www.newport.com/p/F-MBB&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2937,12 +2933,12 @@
         <v>UV curing adhesive</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(implant_data!D5),implant_data!C5,CONCATENATE(" :download:`",implant_data!C5,"&lt;Datasheets/",implant_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C5),"",IF(ISBLANK(implant_data!D5),implant_data!C5,CONCATENATE(" :download:`",implant_data!C5,"&lt;Datasheets/",implant_data!D5,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`NOA 68&lt;Datasheets/uv_adhesive.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK(implant_data!F5),"",CONCATENATE("`",implant_data!E5," &lt;",implant_data!F5,"&gt;`_"))</f>
-        <v>`Norland Products &lt;https://www.norlandproducts2.com/adhesives/adproductsdetail_header_removed.asp?Prdid=68&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F5),"",CONCATENATE("`",implant_data!E5," &lt;",implant_data!F5,"&gt;`__"))</f>
+        <v>`Norland Products &lt;https://www.norlandproducts2.com/adhesives/adproductsdetail_header_removed.asp?Prdid=68&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2955,12 +2951,12 @@
         <v>Ferrule</v>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(implant_data!D6),implant_data!C6,CONCATENATE(" :download:`",implant_data!C6,"&lt;Datasheets/",implant_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C6),"",IF(ISBLANK(implant_data!D6),implant_data!C6,CONCATENATE(" :download:`",implant_data!C6,"&lt;Datasheets/",implant_data!D6,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`MM-FER2007C&lt;Datasheets/ferrule.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(ISBLANK(implant_data!F6),"",CONCATENATE("`",implant_data!E6," &lt;",implant_data!F6,"&gt;`_"))</f>
-        <v>`Precision Fiber Products &lt;https://precisionfiberproducts.com/pfp-lc-1-25mm-od-multimode-ceramic-zirconia-ferrules/&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F6),"",CONCATENATE("`",implant_data!E6," &lt;",implant_data!F6,"&gt;`__"))</f>
+        <v>`Precision Fiber Products &lt;https://precisionfiberproducts.com/pfp-lc-1-25mm-od-multimode-ceramic-zirconia-ferrules/&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2973,12 +2969,12 @@
         <v>Epoxy</v>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(implant_data!D7),implant_data!C7,CONCATENATE(" :download:`",implant_data!C7,"&lt;Datasheets/",implant_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C7),"",IF(ISBLANK(implant_data!D7),implant_data!C7,CONCATENATE(" :download:`",implant_data!C7,"&lt;Datasheets/",implant_data!D7,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`T120023C&lt;Datasheets/epoxy.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(ISBLANK(implant_data!F7),"",CONCATENATE("`",implant_data!E7," &lt;",implant_data!F7,"&gt;`_"))</f>
-        <v>`Fiber Instrument Sales &lt;http://www.fiberinstrumentsales.com/fis-room-cure-epoxy-2-grams.html&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F7),"",CONCATENATE("`",implant_data!E7," &lt;",implant_data!F7,"&gt;`__"))</f>
+        <v>`Fiber Instrument Sales &lt;http://www.fiberinstrumentsales.com/fis-room-cure-epoxy-2-grams.html&gt;`__</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2991,12 +2987,12 @@
         <v>Micro USB vertical socket</v>
       </c>
       <c r="C8" t="str">
-        <f>IF(ISBLANK(implant_data!D8),implant_data!C8,CONCATENATE(" :download:`",implant_data!C8,"&lt;Datasheets/",implant_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C8),"",IF(ISBLANK(implant_data!D8),implant_data!C8,CONCATENATE(" :download:`",implant_data!C8,"&lt;Datasheets/",implant_data!D8,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`1051330011&lt;Datasheets/usb_socket_vertical.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
-        <f>IF(ISBLANK(implant_data!F8),"",CONCATENATE("`",implant_data!E8," &lt;",implant_data!F8,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM10134CT-ND&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F8),"",CONCATENATE("`",implant_data!E8," &lt;",implant_data!F8,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM10134CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3009,12 +3005,12 @@
         <v>Heat shrink tubing</v>
       </c>
       <c r="C9" t="str">
-        <f>IF(ISBLANK(implant_data!D9),implant_data!C9,CONCATENATE(" :download:`",implant_data!C9,"&lt;Datasheets/",implant_data!D9,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C9),"",IF(ISBLANK(implant_data!D9),implant_data!C9,CONCATENATE(" :download:`",implant_data!C9,"&lt;Datasheets/",implant_data!D9,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`HSTTV12-Y&lt;Datasheets/heatshrink.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
-        <f>IF(ISBLANK(implant_data!F9),"",CONCATENATE("`",implant_data!E9," &lt;",implant_data!F9,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=298-11559-ND&gt;`_</v>
+        <f>IF(ISBLANK(implant_data!F9),"",CONCATENATE("`",implant_data!E9," &lt;",implant_data!F9,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=298-11559-ND&gt;`__</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3027,11 +3023,11 @@
         <v xml:space="preserve">0603 10 k\ |OHgr| Resistor </v>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(implant_data!D10),implant_data!C10,CONCATENATE(" :download:`",implant_data!C10,"&lt;Datasheets/",implant_data!D10,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C10),"",IF(ISBLANK(implant_data!D10),implant_data!C10,CONCATENATE(" :download:`",implant_data!C10,"&lt;Datasheets/",implant_data!D10,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D10" t="str">
-        <f>IF(ISBLANK(implant_data!F10),"",CONCATENATE("`",implant_data!E10," &lt;",implant_data!F10,"&gt;`_"))</f>
+        <f>IF(ISBLANK(implant_data!F10),"",CONCATENATE("`",implant_data!E10," &lt;",implant_data!F10,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3045,11 +3041,11 @@
         <v xml:space="preserve">0603 20 k\ |OHgr| Resistor </v>
       </c>
       <c r="C11" t="str">
-        <f>IF(ISBLANK(implant_data!D11),implant_data!C11,CONCATENATE(" :download:`",implant_data!C11,"&lt;Datasheets/",implant_data!D11,"&gt;`"))</f>
+        <f>IF(ISBLANK(implant_data!C11),"",IF(ISBLANK(implant_data!D11),implant_data!C11,CONCATENATE(" :download:`",implant_data!C11,"&lt;Datasheets/",implant_data!D11,"&gt;`")))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D11" t="str">
-        <f>IF(ISBLANK(implant_data!F11),"",CONCATENATE("`",implant_data!E11," &lt;",implant_data!F11,"&gt;`_"))</f>
+        <f>IF(ISBLANK(implant_data!F11),"",CONCATENATE("`",implant_data!E11," &lt;",implant_data!F11,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3071,7 +3067,7 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,7 +3332,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3375,12 +3371,12 @@
         <v>Base Station PCB</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(base_data!C2),"",CONCATENATE(" :download:`",base_data!C2,"&lt;Datasheets/",base_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C2),"",IF(ISBLANK(base_data!D2),base_data!C2,CONCATENATE(" :download:`",base_data!C2,"&lt;Datasheets/",base_data!D2,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`Base Station 2.5&lt;Datasheets/base_station_2.5.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISBLANK(base_data!F2),"",CONCATENATE("`",base_data!E2," &lt;",base_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/qpPpopqr&gt;`_</v>
+        <f>IF(ISBLANK(base_data!F2),"",CONCATENATE("`",base_data!E2," &lt;",base_data!F2,"&gt;`__"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/qpPpopqr&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3393,12 +3389,12 @@
         <v>Feather 32u4 RFM69HCW</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(base_data!C3),"",CONCATENATE(" :download:`",base_data!C3,"&lt;Datasheets/",base_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C3),"",IF(ISBLANK(base_data!D3),base_data!C3,CONCATENATE(" :download:`",base_data!C3,"&lt;Datasheets/",base_data!D3,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`3076&lt;Datasheets/feather_radio.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(ISBLANK(base_data!F3),"",CONCATENATE("`",base_data!E3," &lt;",base_data!F3,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1528-1663-ND&gt;`_</v>
+        <f>IF(ISBLANK(base_data!F3),"",CONCATENATE("`",base_data!E3," &lt;",base_data!F3,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1528-1663-ND&gt;`__</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3411,12 +3407,12 @@
         <v>USB to Serial Converter</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(base_data!C4),"",CONCATENATE(" :download:`",base_data!C4,"&lt;Datasheets/",base_data!D4,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C4),"",IF(ISBLANK(base_data!D4),base_data!C4,CONCATENATE(" :download:`",base_data!C4,"&lt;Datasheets/",base_data!D4,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`CY7C65213-28PVXI&lt;Datasheets/usb_to_serial_converter.pdf&gt;`</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(ISBLANK(base_data!F4),"",CONCATENATE("`",base_data!E4," &lt;",base_data!F4,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09CY7C65213-28PVXI-ND&gt;`_</v>
+        <f>IF(ISBLANK(base_data!F4),"",CONCATENATE("`",base_data!E4," &lt;",base_data!F4,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09CY7C65213-28PVXI-ND&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3429,12 +3425,12 @@
         <v>Voltage Level Translator</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(base_data!C5),"",CONCATENATE(" :download:`",base_data!C5,"&lt;Datasheets/",base_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C5),"",IF(ISBLANK(base_data!D5),base_data!C5,CONCATENATE(" :download:`",base_data!C5,"&lt;Datasheets/",base_data!D5,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`TXB0104PWR&lt;Datasheets/voltage_translator.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK(base_data!F5),"",CONCATENATE("`",base_data!E5," &lt;",base_data!F5,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-21929-1-nd&gt;`_</v>
+        <f>IF(ISBLANK(base_data!F5),"",CONCATENATE("`",base_data!E5," &lt;",base_data!F5,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=296-21929-1-nd&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3447,12 +3443,12 @@
         <v>Micro USB horizontal socket</v>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(base_data!C6),"",CONCATENATE(" :download:`",base_data!C6,"&lt;Datasheets/",base_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C6),"",IF(ISBLANK(base_data!D6),base_data!C6,CONCATENATE(" :download:`",base_data!C6,"&lt;Datasheets/",base_data!D6,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`10118194-0001LF&lt;Datasheets/usb_plug_horizontal.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(ISBLANK(base_data!F6),"",CONCATENATE("`",base_data!E6," &lt;",base_data!F6,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`_</v>
+        <f>IF(ISBLANK(base_data!F6),"",CONCATENATE("`",base_data!E6," &lt;",base_data!F6,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3465,11 +3461,11 @@
         <v xml:space="preserve">0805 51 k\ |OHgr| Resistor </v>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(base_data!C7),"",CONCATENATE(" :download:`",base_data!C7,"&lt;Datasheets/",base_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(base_data!C7),"",IF(ISBLANK(base_data!D7),base_data!C7,CONCATENATE(" :download:`",base_data!C7,"&lt;Datasheets/",base_data!D7,"&gt;`")))</f>
         <v/>
       </c>
       <c r="D7" t="str">
-        <f>IF(ISBLANK(base_data!F7),"",CONCATENATE("`",base_data!E7," &lt;",base_data!F7,"&gt;`_"))</f>
+        <f>IF(ISBLANK(base_data!F7),"",CONCATENATE("`",base_data!E7," &lt;",base_data!F7,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3541,7 +3537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3588,16 +3584,16 @@
         <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3685,7 +3681,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3756,8 +3752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC32778-A014-934E-B9C7-1735DC2E5111}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C2:C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3797,30 +3793,30 @@
         <v>Charging Dock PCB</v>
       </c>
       <c r="C2" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C2),"",CONCATENATE(" :download:`",dock_data!C2,"&lt;Datasheets/",dock_data!D2,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C2),"",IF(ISBLANK(dock_data!D2),dock_data!C2,CONCATENATE(" :download:`",dock_data!C2,"&lt;Datasheets/",dock_data!D2,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`Charging Dock 2.0&lt;Datasheets/charging_dock_2.0.pdf&gt;`</v>
       </c>
       <c r="D2" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F2),"",CONCATENATE("`",dock_data!E2," &lt;",dock_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/hz6upCEq&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F2),"",CONCATENATE("`",dock_data!E2," &lt;",dock_data!F2,"&gt;`__"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/hz6upCEq&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
         <f>TEXT(dock_data!A3,"0")</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>dock_data!B3</f>
-        <v>Molex MicroClasp socket</v>
+        <v>Molex Micro-Lock socket</v>
       </c>
       <c r="C3" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C3),"",CONCATENATE(" :download:`",dock_data!C3,"&lt;Datasheets/",dock_data!D3,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`0559350230&lt;Datasheets/microclasp.pdf&gt;`</v>
+        <f>IF(ISBLANK(dock_data!C3),"",IF(ISBLANK(dock_data!D3),dock_data!C3,CONCATENATE(" :download:`",dock_data!C3,"&lt;Datasheets/",dock_data!D3,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`5055670271&lt;Datasheets/microlock_socket.pdf&gt;`</v>
       </c>
       <c r="D3" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F3),"",CONCATENATE("`",dock_data!E3," &lt;",dock_data!F3,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=wm12296-nd&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F3),"",CONCATENATE("`",dock_data!E3," &lt;",dock_data!F3,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=WM17038CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3833,12 +3829,12 @@
         <v>Lipoly Charging IC</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C4),"",CONCATENATE(" :download:`",dock_data!C4,"&lt;Datasheets/",dock_data!D4,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C4),"",IF(ISBLANK(dock_data!D4),dock_data!C4,CONCATENATE(" :download:`",dock_data!C4,"&lt;Datasheets/",dock_data!D4,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`MCP73831T-2ACI/OT&lt;Datasheets/lipo_charger.pdf&gt;`</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F4),"",CONCATENATE("`",dock_data!E4," &lt;",dock_data!F4,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09MCP73831T-2ACI%2FOTCT-ND&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F4),"",CONCATENATE("`",dock_data!E4," &lt;",dock_data!F4,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=%09MCP73831T-2ACI%2FOTCT-ND&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3851,12 +3847,12 @@
         <v>DC Barrel Power Jack</v>
       </c>
       <c r="C5" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C5),"",CONCATENATE(" :download:`",dock_data!C5,"&lt;Datasheets/",dock_data!D5,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C5),"",IF(ISBLANK(dock_data!D5),dock_data!C5,CONCATENATE(" :download:`",dock_data!C5,"&lt;Datasheets/",dock_data!D5,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`PJ-037A&lt;Datasheets/power_jack.pdf&gt;`</v>
       </c>
       <c r="D5" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F5),"",CONCATENATE("`",dock_data!E5," &lt;",dock_data!F5,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=cp-037a-nd&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F5),"",CONCATENATE("`",dock_data!E5," &lt;",dock_data!F5,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=cp-037a-nd&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3869,12 +3865,12 @@
         <v>5V 2.5A Power Supply</v>
       </c>
       <c r="C6" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C6),"",CONCATENATE(" :download:`",dock_data!C6,"&lt;Datasheets/",dock_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C6),"",IF(ISBLANK(dock_data!D6),dock_data!C6,CONCATENATE(" :download:`",dock_data!C6,"&lt;Datasheets/",dock_data!D6,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`SWI12-5-N-P5R&lt;Datasheets/power_supply.pdf&gt;`</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F6),"",CONCATENATE("`",dock_data!E6," &lt;",dock_data!F6,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/cui-inc/SWI12-5-N-P5R/102-3425-ND/5287234&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F6),"",CONCATENATE("`",dock_data!E6," &lt;",dock_data!F6,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/cui-inc/SWI12-5-N-P5R/102-3425-ND/5287234&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3887,12 +3883,12 @@
         <v>Green LED</v>
       </c>
       <c r="C7" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C7),"",CONCATENATE(" :download:`",dock_data!C7,"&lt;Datasheets/",dock_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C7),"",IF(ISBLANK(dock_data!D7),dock_data!C7,CONCATENATE(" :download:`",dock_data!C7,"&lt;Datasheets/",dock_data!D7,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`151031VS06000&lt;Datasheets/led_3mm_green.pdf&gt;`</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F7),"",CONCATENATE("`",dock_data!E7," &lt;",dock_data!F7,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5008-ND&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F7),"",CONCATENATE("`",dock_data!E7," &lt;",dock_data!F7,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5008-ND&gt;`__</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3905,12 +3901,12 @@
         <v>Red LED</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C8),"",CONCATENATE(" :download:`",dock_data!C8,"&lt;Datasheets/",dock_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C8),"",IF(ISBLANK(dock_data!D8),dock_data!C8,CONCATENATE(" :download:`",dock_data!C8,"&lt;Datasheets/",dock_data!D8,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`151031SS06000&lt;Datasheets/led_3mm_red.pdf&gt;`</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F8),"",CONCATENATE("`",dock_data!E8," &lt;",dock_data!F8,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5006-ND&gt;`_</v>
+        <f>IF(ISBLANK(dock_data!F8),"",CONCATENATE("`",dock_data!E8," &lt;",dock_data!F8,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=732-5006-ND&gt;`__</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3923,11 +3919,11 @@
         <v xml:space="preserve">0805 470 \ |OHgr| Resistor </v>
       </c>
       <c r="C9" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C9),"",CONCATENATE(" :download:`",dock_data!C9,"&lt;Datasheets/",dock_data!D9,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C9),"",IF(ISBLANK(dock_data!D9),dock_data!C9,CONCATENATE(" :download:`",dock_data!C9,"&lt;Datasheets/",dock_data!D9,"&gt;`")))</f>
         <v/>
       </c>
       <c r="D9" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F9),"",CONCATENATE("`",dock_data!E9," &lt;",dock_data!F9,"&gt;`_"))</f>
+        <f>IF(ISBLANK(dock_data!F9),"",CONCATENATE("`",dock_data!E9," &lt;",dock_data!F9,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3941,11 +3937,11 @@
         <v xml:space="preserve">0805 2.5 K\ |OHgr| Resistor </v>
       </c>
       <c r="C10" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C10),"",CONCATENATE(" :download:`",dock_data!C10,"&lt;Datasheets/",dock_data!D10,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C10),"",IF(ISBLANK(dock_data!D10),dock_data!C10,CONCATENATE(" :download:`",dock_data!C10,"&lt;Datasheets/",dock_data!D10,"&gt;`")))</f>
         <v/>
       </c>
       <c r="D10" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F10),"",CONCATENATE("`",dock_data!E10," &lt;",dock_data!F10,"&gt;`_"))</f>
+        <f>IF(ISBLANK(dock_data!F10),"",CONCATENATE("`",dock_data!E10," &lt;",dock_data!F10,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3959,11 +3955,11 @@
         <v>0805 10 |mgr|\F Capacitor</v>
       </c>
       <c r="C11" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!C11),"",CONCATENATE(" :download:`",dock_data!C11,"&lt;Datasheets/",dock_data!D11,"&gt;`"))</f>
+        <f>IF(ISBLANK(dock_data!C11),"",IF(ISBLANK(dock_data!D11),dock_data!C11,CONCATENATE(" :download:`",dock_data!C11,"&lt;Datasheets/",dock_data!D11,"&gt;`")))</f>
         <v/>
       </c>
       <c r="D11" s="7" t="str">
-        <f>IF(ISBLANK(dock_data!F11),"",CONCATENATE("`",dock_data!E11," &lt;",dock_data!F11,"&gt;`_"))</f>
+        <f>IF(ISBLANK(dock_data!F11),"",CONCATENATE("`",dock_data!E11," &lt;",dock_data!F11,"&gt;`__"))</f>
         <v/>
       </c>
     </row>
@@ -3982,7 +3978,7 @@
   <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4025,59 +4021,59 @@
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>129</v>
+        <v>248</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4085,19 +4081,19 @@
         <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4105,67 +4101,67 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4174,10 +4170,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4186,10 +4182,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -4246,7 +4242,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4286,12 +4282,12 @@
         <v>Programmer PCB</v>
       </c>
       <c r="C2" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C2),"",CONCATENATE(" :download:`",programmer_data!C2,"&lt;Datasheets/",programmer_data!D2,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`Cerebro ICSP 1.2&lt;Datasheets/&gt;`</v>
+        <f>IF(ISBLANK(programmer_data!C2),"",IF(ISBLANK(programmer_data!D2),programmer_data!C2,CONCATENATE(" :download:`",programmer_data!C2,"&lt;Datasheets/",programmer_data!D2,"&gt;`")))</f>
+        <v>Cerebro ICSP 1.2</v>
       </c>
       <c r="D2" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F2),"",CONCATENATE("`",programmer_data!E2," &lt;",programmer_data!F2,"&gt;`_"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/PXMM4F8R&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F2),"",CONCATENATE("`",programmer_data!E2," &lt;",programmer_data!F2,"&gt;`__"))</f>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/PXMM4F8R&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,12 +4300,12 @@
         <v>6 Pin Socket</v>
       </c>
       <c r="C3" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C3),"",CONCATENATE(" :download:`",programmer_data!C3,"&lt;Datasheets/",programmer_data!D3,"&gt;`"))</f>
+        <f>IF(ISBLANK(programmer_data!C3),"",IF(ISBLANK(programmer_data!D3),programmer_data!C3,CONCATENATE(" :download:`",programmer_data!C3,"&lt;Datasheets/",programmer_data!D3,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`75869-331LF&lt;Datasheets/ICSP_socket.pdf&gt;`</v>
       </c>
       <c r="D3" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F3),"",CONCATENATE("`",programmer_data!E3," &lt;",programmer_data!F3,"&gt;`_"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-5122-ND&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F3),"",CONCATENATE("`",programmer_data!E3," &lt;",programmer_data!F3,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-5122-ND&gt;`__</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4322,12 +4318,12 @@
         <v>Spear Head Pogo Pin</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C4),"",CONCATENATE(" :download:`",programmer_data!C4,"&lt;Datasheets/",programmer_data!D4,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`394&lt;Datasheets/&gt;`</v>
+        <f>IF(ISBLANK(programmer_data!C4),"",IF(ISBLANK(programmer_data!D4),programmer_data!C4,CONCATENATE(" :download:`",programmer_data!C4,"&lt;Datasheets/",programmer_data!D4,"&gt;`")))</f>
+        <v>394</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F4),"",CONCATENATE("`",programmer_data!E4," &lt;",programmer_data!F4,"&gt;`_"))</f>
-        <v>`Adafruit &lt;https://www.adafruit.com/product/394&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F4),"",CONCATENATE("`",programmer_data!E4," &lt;",programmer_data!F4,"&gt;`__"))</f>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/394&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4340,12 +4336,12 @@
         <v>Needle Head Pogo Pin</v>
       </c>
       <c r="C5" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C5),"",CONCATENATE(" :download:`",programmer_data!C5,"&lt;Datasheets/",programmer_data!D5,"&gt;`"))</f>
-        <v xml:space="preserve"> :download:`2430&lt;Datasheets/&gt;`</v>
+        <f>IF(ISBLANK(programmer_data!C5),"",IF(ISBLANK(programmer_data!D5),programmer_data!C5,CONCATENATE(" :download:`",programmer_data!C5,"&lt;Datasheets/",programmer_data!D5,"&gt;`")))</f>
+        <v>2430</v>
       </c>
       <c r="D5" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F5),"",CONCATENATE("`",programmer_data!E5," &lt;",programmer_data!F5,"&gt;`_"))</f>
-        <v>`Adafruit &lt;https://www.adafruit.com/product/2430&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F5),"",CONCATENATE("`",programmer_data!E5," &lt;",programmer_data!F5,"&gt;`__"))</f>
+        <v>`Adafruit &lt;https://www.adafruit.com/product/2430&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4358,12 +4354,12 @@
         <v>M3 x 0.5 Screw</v>
       </c>
       <c r="C6" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C6),"",CONCATENATE(" :download:`",programmer_data!C6,"&lt;Datasheets/",programmer_data!D6,"&gt;`"))</f>
+        <f>IF(ISBLANK(programmer_data!C6),"",IF(ISBLANK(programmer_data!D6),programmer_data!C6,CONCATENATE(" :download:`",programmer_data!C6,"&lt;Datasheets/",programmer_data!D6,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`92492A717&lt;Datasheets/m3_nylon_screw.pdf&gt;`</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F6),"",CONCATENATE("`",programmer_data!E6," &lt;",programmer_data!F6,"&gt;`_"))</f>
-        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#92492A717&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F6),"",CONCATENATE("`",programmer_data!E6," &lt;",programmer_data!F6,"&gt;`__"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#92492A717&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4376,12 +4372,12 @@
         <v>Nylon Spacer</v>
       </c>
       <c r="C7" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C7),"",CONCATENATE(" :download:`",programmer_data!C7,"&lt;Datasheets/",programmer_data!D7,"&gt;`"))</f>
+        <f>IF(ISBLANK(programmer_data!C7),"",IF(ISBLANK(programmer_data!D7),programmer_data!C7,CONCATENATE(" :download:`",programmer_data!C7,"&lt;Datasheets/",programmer_data!D7,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`93657A203&lt;Datasheets/nylon_spacer.pdf&gt;`</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F7),"",CONCATENATE("`",programmer_data!E7," &lt;",programmer_data!F7,"&gt;`_"))</f>
-        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#93657A203&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F7),"",CONCATENATE("`",programmer_data!E7," &lt;",programmer_data!F7,"&gt;`__"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#93657A203&gt;`__</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4394,12 +4390,12 @@
         <v>M3 Nut</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!C8),"",CONCATENATE(" :download:`",programmer_data!C8,"&lt;Datasheets/",programmer_data!D8,"&gt;`"))</f>
+        <f>IF(ISBLANK(programmer_data!C8),"",IF(ISBLANK(programmer_data!D8),programmer_data!C8,CONCATENATE(" :download:`",programmer_data!C8,"&lt;Datasheets/",programmer_data!D8,"&gt;`")))</f>
         <v xml:space="preserve"> :download:`90695A033&lt;Datasheets/m3_nut.pdf&gt;`</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f>IF(ISBLANK(programmer_data!F8),"",CONCATENATE("`",programmer_data!E8," &lt;",programmer_data!F8,"&gt;`_"))</f>
-        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#90695A033&gt;`_</v>
+        <f>IF(ISBLANK(programmer_data!F8),"",CONCATENATE("`",programmer_data!E8," &lt;",programmer_data!F8,"&gt;`__"))</f>
+        <v>`McMaster-Carr &lt;https://www.mcmaster.com/#90695A033&gt;`__</v>
       </c>
     </row>
     <row r="51" spans="4:4" hidden="1" x14ac:dyDescent="0.2"/>

</xml_diff>